<commit_message>
Descripció constructiva de tots els sistemes de l'edifici en la generació del Word
</commit_message>
<xml_diff>
--- a/lib/documents_treball/operacions_manteniment_v2.xlsx
+++ b/lib/documents_treball/operacions_manteniment_v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Operacions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4525" uniqueCount="1675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1980">
   <si>
     <t>sistema</t>
   </si>
@@ -5050,6 +5050,921 @@
   </si>
   <si>
     <t>Limpieza de las barandillas interiores.</t>
+  </si>
+  <si>
+    <t>no_sistema_evacuacio</t>
+  </si>
+  <si>
+    <t>No disposa de sistema d'evacuació</t>
+  </si>
+  <si>
+    <t>si_sistema_evacuacio</t>
+  </si>
+  <si>
+    <t>Disposa de sistema d'evacuació</t>
+  </si>
+  <si>
+    <t>fosa_septica</t>
+  </si>
+  <si>
+    <t>Disposa de sistema d'evacuació propi (fossa sèptica, etc.)</t>
+  </si>
+  <si>
+    <t>colectors_vistos</t>
+  </si>
+  <si>
+    <t>Els col·lectors són vistos</t>
+  </si>
+  <si>
+    <t>bomba_elevacio</t>
+  </si>
+  <si>
+    <t>Disposa de bomba d'elevació</t>
+  </si>
+  <si>
+    <t>separador_greixos</t>
+  </si>
+  <si>
+    <t>Disposa de separador de greixos i fangs</t>
+  </si>
+  <si>
+    <t>baixants_vistos</t>
+  </si>
+  <si>
+    <t>Baixants vistos</t>
+  </si>
+  <si>
+    <t>baixants_encastats</t>
+  </si>
+  <si>
+    <t>Baixants encastats</t>
+  </si>
+  <si>
+    <t>baixants_ceramics</t>
+  </si>
+  <si>
+    <t>Baixants ceràmics</t>
+  </si>
+  <si>
+    <t>baixants_pvc</t>
+  </si>
+  <si>
+    <t>Baixants de PVC</t>
+  </si>
+  <si>
+    <t>baixants_fibrociment</t>
+  </si>
+  <si>
+    <t>Baixants de fibrociment</t>
+  </si>
+  <si>
+    <t>baixants_coure</t>
+  </si>
+  <si>
+    <t>Baixants de coure</t>
+  </si>
+  <si>
+    <t>baixants_alumini</t>
+  </si>
+  <si>
+    <t>Baixants d'alumini</t>
+  </si>
+  <si>
+    <t>baixants_polipropile</t>
+  </si>
+  <si>
+    <t>Baixants de polipropilè</t>
+  </si>
+  <si>
+    <t>baixants_zinc</t>
+  </si>
+  <si>
+    <t>Baixants de zinc</t>
+  </si>
+  <si>
+    <t>Col·lectors vistos</t>
+  </si>
+  <si>
+    <t>colectors_soterrats</t>
+  </si>
+  <si>
+    <t>Col·lectors soterrats</t>
+  </si>
+  <si>
+    <t>colectors_formigo</t>
+  </si>
+  <si>
+    <t>Col·lectors de formigó</t>
+  </si>
+  <si>
+    <t>colectors_ceramic</t>
+  </si>
+  <si>
+    <t>Col·lectors ceràmics</t>
+  </si>
+  <si>
+    <t>colectors_fibrociment</t>
+  </si>
+  <si>
+    <t>Col·lectors de fibrociment</t>
+  </si>
+  <si>
+    <t>colectors_pvc</t>
+  </si>
+  <si>
+    <t>Col·lectors de PVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No dispone de sistema de evacuación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dispone de sistema de evacuación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dispone de sistema de evacuación propio (fosa séptica, etc.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los colectors son vistos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dispone de bomba de elevación</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dispone de separador de grasas y barros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes vistos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes encastados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes cerámicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de PVC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de fibrocemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de cobre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de aluminio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de polipropileno</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bajantes de zinc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores vistos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores enterrados</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores de hormigón</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores cerámicos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores de fibrocemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Colectores de PVC</t>
+  </si>
+  <si>
+    <t>connexio_directa</t>
+  </si>
+  <si>
+    <t>Dispone de conexión directa a red pública de suministro de agua</t>
+  </si>
+  <si>
+    <t>connexio_aforament</t>
+  </si>
+  <si>
+    <t>Dispone de conexión por aforo a red pública de suministro de agua</t>
+  </si>
+  <si>
+    <t>captacio_propia</t>
+  </si>
+  <si>
+    <t>Dispone de captación propia (pozo, bomba, etc.)</t>
+  </si>
+  <si>
+    <t>grup_pressio</t>
+  </si>
+  <si>
+    <t>Dispone de grupo de presión</t>
+  </si>
+  <si>
+    <t>comptador_unic</t>
+  </si>
+  <si>
+    <t>Contador único para todo el edificio</t>
+  </si>
+  <si>
+    <t>comptadors_individuals_habitatge</t>
+  </si>
+  <si>
+    <t>Contadores individuales por vivienda/local</t>
+  </si>
+  <si>
+    <t>comptadors_individuals_centralitzats</t>
+  </si>
+  <si>
+    <t>Contadores individuales centralizados</t>
+  </si>
+  <si>
+    <t>muntants_plom</t>
+  </si>
+  <si>
+    <t>muntants_ferro</t>
+  </si>
+  <si>
+    <t>muntants_coure</t>
+  </si>
+  <si>
+    <t>muntants_plastic</t>
+  </si>
+  <si>
+    <t>Disposa de connexió directa a xarxa pública de subministrament d'aigua</t>
+  </si>
+  <si>
+    <t>Disposa de connexió per aforament a xarxa pública de subministrament d'aigua</t>
+  </si>
+  <si>
+    <t>Disposa de captació pròpia (pou, bomba, etc.)</t>
+  </si>
+  <si>
+    <t>Disposa de grup de pressió</t>
+  </si>
+  <si>
+    <t>Comptador únic per tot l'edifici</t>
+  </si>
+  <si>
+    <t>Comptadors individuals per habitatge/local</t>
+  </si>
+  <si>
+    <t>Comptadors individuals centralitzats</t>
+  </si>
+  <si>
+    <t>Muntants de plom</t>
+  </si>
+  <si>
+    <t>Muntants de ferro</t>
+  </si>
+  <si>
+    <t>Muntants de coure</t>
+  </si>
+  <si>
+    <t>Muntants de plàstic</t>
+  </si>
+  <si>
+    <t>Montantes de plomo</t>
+  </si>
+  <si>
+    <t>Montantes de hierro</t>
+  </si>
+  <si>
+    <t>Montantes de cobre</t>
+  </si>
+  <si>
+    <t>Montantes de plástico</t>
+  </si>
+  <si>
+    <t>enllumenat_comunitari</t>
+  </si>
+  <si>
+    <t>Dispone de alumbrado comunitario</t>
+  </si>
+  <si>
+    <t>mes_100k</t>
+  </si>
+  <si>
+    <t>Potencia total instalada superior a los 100 kW</t>
+  </si>
+  <si>
+    <t>connexio_terra</t>
+  </si>
+  <si>
+    <t>Dispone de conexión a tierra</t>
+  </si>
+  <si>
+    <t>centre_transformacio</t>
+  </si>
+  <si>
+    <t>Hay un centro de transformación en el edificio</t>
+  </si>
+  <si>
+    <t>fotovoltaica</t>
+  </si>
+  <si>
+    <t>Dispone de instalación solar fotovoltaica</t>
+  </si>
+  <si>
+    <t>Disposa d'enllumenat comunitari</t>
+  </si>
+  <si>
+    <t>Potència total instal·lada superior als 100 kW</t>
+  </si>
+  <si>
+    <t>Disposa de connexió a terra</t>
+  </si>
+  <si>
+    <t>Hi ha un centre de transformació a l'edifici</t>
+  </si>
+  <si>
+    <t>Disposa d'instal·lació solar fotovoltaica</t>
+  </si>
+  <si>
+    <t>escalfador_pn_menor_24</t>
+  </si>
+  <si>
+    <t>escalfador_pn_24_70</t>
+  </si>
+  <si>
+    <t>escalfador_pn_major_70</t>
+  </si>
+  <si>
+    <t>caldera_gas_pn_menor_70</t>
+  </si>
+  <si>
+    <t>Caldera a gas Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>caldera_gas_pn_major_70</t>
+  </si>
+  <si>
+    <t>Caldera a gas Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>caldera_biomassa</t>
+  </si>
+  <si>
+    <t>Caldera a biomasa</t>
+  </si>
+  <si>
+    <t>caldera_solar_termica</t>
+  </si>
+  <si>
+    <t>Caldera o calentador con instalación de energía solar térmica</t>
+  </si>
+  <si>
+    <t>altres_pn_menor_70</t>
+  </si>
+  <si>
+    <t>altres_pn_major_70</t>
+  </si>
+  <si>
+    <t>clima_pn_menor_12_autonoms</t>
+  </si>
+  <si>
+    <t>clima_pn_menor_12_torres</t>
+  </si>
+  <si>
+    <t>clima_pn_menor_12_recuperador</t>
+  </si>
+  <si>
+    <t>clima_pn_12_70_autonoms</t>
+  </si>
+  <si>
+    <t>clima_pn_12_70_torres</t>
+  </si>
+  <si>
+    <t>clima_pn_12_70_recuperador</t>
+  </si>
+  <si>
+    <t>clima_pn_major_70_autonoms</t>
+  </si>
+  <si>
+    <t>clima_pn_major_70_torres</t>
+  </si>
+  <si>
+    <t>clima_pn_major_70_recuperador</t>
+  </si>
+  <si>
+    <t>Caldera a biomassa</t>
+  </si>
+  <si>
+    <t>Caldera o escalfador amb instal·lació d’energia solar tèrmica</t>
+  </si>
+  <si>
+    <t>Escalfador Pn ≤ 24,4 kW</t>
+  </si>
+  <si>
+    <t>Escalfador 24,4 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Escalfador Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Calentador Pn ≤ 24,4 kW</t>
+  </si>
+  <si>
+    <t>Calentador 24,4 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Calentador Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Caldera Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Caldera Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització autònom Pn ≤ 12 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb torre de refrigeració Pn ≤ 12 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización autónomo Pn ≤ 12 kW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema de climatización con torre de refrigeración Pn ≤ 12 kW </t>
+  </si>
+  <si>
+    <t>Sistema de climatización con recuperación de calor Pn ≤ 12 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització autònom 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització autònom Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb torre de refrigeració 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb torre de refrigeració Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb recuperació de calor Pn ≤ 12 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb recuperació de calor 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb recuperació de calor Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización autónomo 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con torre de refrigeración 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con torre de refrigeración Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización autónomo Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con recuperación de calor 12 kW &lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con recuperación de calor Pn &gt; 70 kW</t>
+  </si>
+  <si>
+    <t>instalacio_gas</t>
+  </si>
+  <si>
+    <t>Acometida a red de distribución canalizada de gas para uso doméstico</t>
+  </si>
+  <si>
+    <t>diposit_aire_lliure</t>
+  </si>
+  <si>
+    <t>diposit_enterrat</t>
+  </si>
+  <si>
+    <t>Depósito de gas propano al aire libre</t>
+  </si>
+  <si>
+    <t>Depósito de gas propano enterrado</t>
+  </si>
+  <si>
+    <t>Escomesa a xarxa de distribució canalitzada de gas per a ús domèstic</t>
+  </si>
+  <si>
+    <t>Dipòsit de gas propà a l'aire lliure</t>
+  </si>
+  <si>
+    <t>Dipòsit de gas propà enterrat</t>
+  </si>
+  <si>
+    <t>habitatge_natural_conductes</t>
+  </si>
+  <si>
+    <t>Natural por conductos</t>
+  </si>
+  <si>
+    <t>habitatge_natural_obertures</t>
+  </si>
+  <si>
+    <t>Natural por aperturas</t>
+  </si>
+  <si>
+    <t>habitatge_mecanica_conductes</t>
+  </si>
+  <si>
+    <t>Mecánica por conductos</t>
+  </si>
+  <si>
+    <t>habitatge_mecanica_obertures</t>
+  </si>
+  <si>
+    <t>Mecánica por aperturas</t>
+  </si>
+  <si>
+    <t>habitatge_mecanica_control</t>
+  </si>
+  <si>
+    <t>Mecánica con sistema de control</t>
+  </si>
+  <si>
+    <t>traster_natural_conductes</t>
+  </si>
+  <si>
+    <t>traster_natural_obertures</t>
+  </si>
+  <si>
+    <t>traster_mecanica_conductes</t>
+  </si>
+  <si>
+    <t>traster_mecanica_obertures</t>
+  </si>
+  <si>
+    <t>traster_mecanica_control</t>
+  </si>
+  <si>
+    <t>magatzem_natural_conductes</t>
+  </si>
+  <si>
+    <t>magatzem_natural_obertures</t>
+  </si>
+  <si>
+    <t>magatzem_mecanica_conductes</t>
+  </si>
+  <si>
+    <t>magatzem_mecanica_obertures</t>
+  </si>
+  <si>
+    <t>magatzem_mecanica_control</t>
+  </si>
+  <si>
+    <t>garatge_natural_conductes</t>
+  </si>
+  <si>
+    <t>garatge_natural_obertures</t>
+  </si>
+  <si>
+    <t>garatge_mecanica_conductes</t>
+  </si>
+  <si>
+    <t>garatge_mecanica_obertures</t>
+  </si>
+  <si>
+    <t>garatge_mecanica_control</t>
+  </si>
+  <si>
+    <t>Natural per conductes</t>
+  </si>
+  <si>
+    <t>Natural per obertures</t>
+  </si>
+  <si>
+    <t>Mecànica per conductes</t>
+  </si>
+  <si>
+    <t>Mecànica per obertures</t>
+  </si>
+  <si>
+    <t>Mecànica amb sistema de control</t>
+  </si>
+  <si>
+    <t>alarma_automatica</t>
+  </si>
+  <si>
+    <t>Sistema automático de detección y alarma de incendios</t>
+  </si>
+  <si>
+    <t>alarma_manual</t>
+  </si>
+  <si>
+    <t>Sistema manual de alarma de incendios</t>
+  </si>
+  <si>
+    <t>extintors</t>
+  </si>
+  <si>
+    <t>Extintores de incendios</t>
+  </si>
+  <si>
+    <t>abastiment_aigua</t>
+  </si>
+  <si>
+    <t>Sistema de suministro de agua contra incendios</t>
+  </si>
+  <si>
+    <t>bie</t>
+  </si>
+  <si>
+    <t>Boca de incendios equipada (BIE)</t>
+  </si>
+  <si>
+    <t>hidrants</t>
+  </si>
+  <si>
+    <t>Hidrantes</t>
+  </si>
+  <si>
+    <t>ruixadors</t>
+  </si>
+  <si>
+    <t>Sistema fijo de extinción (rociadores)</t>
+  </si>
+  <si>
+    <t>columnes_seques</t>
+  </si>
+  <si>
+    <t>Columnas secas</t>
+  </si>
+  <si>
+    <t>parallamps</t>
+  </si>
+  <si>
+    <t>Pararayos</t>
+  </si>
+  <si>
+    <t>Sistema automàtic de detecció i alarma d’incendis</t>
+  </si>
+  <si>
+    <t>Sistema manual d’alarma d’incendis</t>
+  </si>
+  <si>
+    <t>Extintors d’incendis</t>
+  </si>
+  <si>
+    <t>Sistema d’abastiment d’aigua contra incendis</t>
+  </si>
+  <si>
+    <t>Boca d’incendis equipada (BIE)</t>
+  </si>
+  <si>
+    <t>Hidrants</t>
+  </si>
+  <si>
+    <t>Sistemes fixes d’extinció (ruixadors)</t>
+  </si>
+  <si>
+    <t>Columnes seques</t>
+  </si>
+  <si>
+    <t>Parallamps</t>
+  </si>
+  <si>
+    <t>habitatge_unifamiliar</t>
+  </si>
+  <si>
+    <t>edifici_comunitari</t>
+  </si>
+  <si>
+    <t>Ascensor en edificio comunitario de uso residencial de hasta seis paradas, con antigüedad menor de 20 años</t>
+  </si>
+  <si>
+    <t>mes_20_plantes</t>
+  </si>
+  <si>
+    <t>altres</t>
+  </si>
+  <si>
+    <t>La vivienda dispone de ascensor</t>
+  </si>
+  <si>
+    <t>Ascensor instalado en edificios de más de 20 viviendas, o con más de 4 plantas servidas</t>
+  </si>
+  <si>
+    <t>Ascensor</t>
+  </si>
+  <si>
+    <t>Ascensor en edifici comunitari d’ús residencial de fins a sis parades, amb antiguitat menor de 20 anys</t>
+  </si>
+  <si>
+    <t>Ascensor instal·lat en edifici de més de 20 habitatges, o amb més de 4 plantes servides</t>
+  </si>
+  <si>
+    <t>L'habitatge disposa d'ascensor</t>
+  </si>
+  <si>
+    <t>ascensors</t>
+  </si>
+  <si>
+    <t>porter_audio</t>
+  </si>
+  <si>
+    <t>Portero electrónico con sistema de audio</t>
+  </si>
+  <si>
+    <t>porter_video</t>
+  </si>
+  <si>
+    <t>Portero electrónico con sistema de audio y vídeo</t>
+  </si>
+  <si>
+    <t>antena_individual</t>
+  </si>
+  <si>
+    <t>Antena individual y red coaxial</t>
+  </si>
+  <si>
+    <t>antena_colectiva</t>
+  </si>
+  <si>
+    <t>Antena colectiva y red coaxial</t>
+  </si>
+  <si>
+    <t>parabolica_individual</t>
+  </si>
+  <si>
+    <t>Antena parabólica individual</t>
+  </si>
+  <si>
+    <t>parabolica_colectiva</t>
+  </si>
+  <si>
+    <t>Antena parabólica colectiva</t>
+  </si>
+  <si>
+    <t>telefonia</t>
+  </si>
+  <si>
+    <t>Instalación de telefonía</t>
+  </si>
+  <si>
+    <t>riti</t>
+  </si>
+  <si>
+    <t>RITI (Recinto de instalaciones de telecomunicaciones inferior)</t>
+  </si>
+  <si>
+    <t>rits</t>
+  </si>
+  <si>
+    <t>RITS (Recinto de instalaciones de telecomunicaciones superior)</t>
+  </si>
+  <si>
+    <t>ritu</t>
+  </si>
+  <si>
+    <t>RITU (Recinto de instalaciones de telecomunicaciones único)</t>
+  </si>
+  <si>
+    <t>ritm</t>
+  </si>
+  <si>
+    <t>RITM (Recinto de instalaciones de telecomunicaciones único modular prefabricado)</t>
+  </si>
+  <si>
+    <t>Porter electrònic amb sistema d'àudio</t>
+  </si>
+  <si>
+    <t>Porter electrònic amb sistema d'àudio i vídeo</t>
+  </si>
+  <si>
+    <t>Antena individual i xarxa coaxial</t>
+  </si>
+  <si>
+    <t>Antena col·lectiva i xarxa coaxial</t>
+  </si>
+  <si>
+    <t>Antena parabòlica individual</t>
+  </si>
+  <si>
+    <t>Antena parabòlica col·lectiva</t>
+  </si>
+  <si>
+    <t>Instal·lació de telefonia</t>
+  </si>
+  <si>
+    <t>RITI (Recinte d’instal·lacions de telecomunicacions inferior)</t>
+  </si>
+  <si>
+    <t>RITS (Recinte d’instal·lacions de telecomunicacions superior)</t>
+  </si>
+  <si>
+    <t>RITU (Recinte d’instal·lacions de telecomunicacions únic)</t>
+  </si>
+  <si>
+    <t>RITM (Recinte d’instal·lacions de telecomunicacions únic modular prefabricat)</t>
+  </si>
+  <si>
+    <t>piscina_estructura_obra</t>
+  </si>
+  <si>
+    <t>piscina_estructura_composite</t>
+  </si>
+  <si>
+    <t>piscina_estructura_acer</t>
+  </si>
+  <si>
+    <t>piscina_vores_formigo</t>
+  </si>
+  <si>
+    <t>Bordes prefabricados de hormigón</t>
+  </si>
+  <si>
+    <t>piscina_vores_pedra</t>
+  </si>
+  <si>
+    <t>Bordes de piedra natural</t>
+  </si>
+  <si>
+    <t>piscina_ceramica</t>
+  </si>
+  <si>
+    <t>Revestimiento de piezas cerámicas</t>
+  </si>
+  <si>
+    <t>piscina_resines</t>
+  </si>
+  <si>
+    <t>Revestimiento de resinas sintéticas</t>
+  </si>
+  <si>
+    <t>piscina_porcellana</t>
+  </si>
+  <si>
+    <t>Revestimiento de porcelana</t>
+  </si>
+  <si>
+    <t>piscina_climatitzacio</t>
+  </si>
+  <si>
+    <t>Dispone de instalación de climatización</t>
+  </si>
+  <si>
+    <t>piscina_iluminacio</t>
+  </si>
+  <si>
+    <t>Dispone de instalación de iluminación sumergida</t>
+  </si>
+  <si>
+    <t>piscina_purificador</t>
+  </si>
+  <si>
+    <t>Dispone de instalación de purificación de aguas</t>
+  </si>
+  <si>
+    <t>Vores prefabricades de formigó</t>
+  </si>
+  <si>
+    <t>Vores de pedra natural</t>
+  </si>
+  <si>
+    <t>Revestiment de peces ceràmiques</t>
+  </si>
+  <si>
+    <t>Revestiment de resines sintètiques</t>
+  </si>
+  <si>
+    <t>Revestiment de porcellana</t>
+  </si>
+  <si>
+    <t>Disposa d'instal·lació de climatització</t>
+  </si>
+  <si>
+    <t>Disposa d'instal·lació d'il·luminació submergida</t>
+  </si>
+  <si>
+    <t>Disposa d'instal·lació de purificació d'aigües</t>
+  </si>
+  <si>
+    <t>Piscina amb estructura d'obra</t>
+  </si>
+  <si>
+    <t>Piscina amb estructura de materials composites</t>
+  </si>
+  <si>
+    <t>Piscina amb estructura d'acer</t>
+  </si>
+  <si>
+    <t>Piscina con estructura de obra</t>
+  </si>
+  <si>
+    <t>Piscina con estructura de materiales composites</t>
+  </si>
+  <si>
+    <t>Piscina con estructura de acero</t>
+  </si>
+  <si>
+    <t>º</t>
   </si>
 </sst>
 </file>
@@ -5460,7 +6375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N419"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
+    <sheetView topLeftCell="A392" workbookViewId="0">
       <selection activeCell="B409" sqref="B409:B419"/>
     </sheetView>
   </sheetViews>
@@ -23265,16 +24180,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F288"/>
+  <dimension ref="A1:F406"/>
   <sheetViews>
-    <sheetView topLeftCell="A273" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F288" sqref="F2:F288"/>
+    <sheetView tabSelected="1" topLeftCell="A383" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F406" sqref="F406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" customWidth="1"/>
   </cols>
@@ -26781,7 +27696,7 @@
         <v>1167</v>
       </c>
       <c r="F195" t="str">
-        <f t="shared" ref="F195:F288" si="3">"ElementPredefinit.create(nom_element: """&amp;B195&amp;""", sistema_element: """&amp;A195&amp;""", descripcio_ca: """&amp;C195&amp;""", descripcio_es: """&amp;D195&amp;""")"</f>
+        <f t="shared" ref="F195:F289" si="3">"ElementPredefinit.create(nom_element: """&amp;B195&amp;""", sistema_element: """&amp;A195&amp;""", descripcio_ca: """&amp;C195&amp;""", descripcio_es: """&amp;D195&amp;""")"</f>
         <v>ElementPredefinit.create(nom_element: "aillament_plaques", sistema_element: "coberta", descripcio_ca: "Foma de l'aïllament: plaques", descripcio_es: "Forma del aislamiento: placas")</v>
       </c>
     </row>
@@ -28457,6 +29372,2099 @@
       <c r="F288" t="str">
         <f t="shared" si="3"/>
         <v>ElementPredefinit.create(nom_element: "barana_metacrilat", sistema_element: "particions", descripcio_ca: "Baranes de metacrilat", descripcio_es: "Barandillas de metacrilato")</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>179</v>
+      </c>
+      <c r="B289" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C289" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D289" t="s">
+        <v>1716</v>
+      </c>
+      <c r="F289" t="str">
+        <f t="shared" si="3"/>
+        <v>ElementPredefinit.create(nom_element: "no_sistema_evacuacio", sistema_element: "sanejament", descripcio_ca: "No disposa de sistema d'evacuació", descripcio_es: " No dispone de sistema de evacuación")</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>179</v>
+      </c>
+      <c r="B290" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C290" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D290" t="s">
+        <v>1717</v>
+      </c>
+      <c r="F290" t="str">
+        <f t="shared" ref="F290:F353" si="4">"ElementPredefinit.create(nom_element: """&amp;B290&amp;""", sistema_element: """&amp;A290&amp;""", descripcio_ca: """&amp;C290&amp;""", descripcio_es: """&amp;D290&amp;""")"</f>
+        <v>ElementPredefinit.create(nom_element: "si_sistema_evacuacio", sistema_element: "sanejament", descripcio_ca: "Disposa de sistema d'evacuació", descripcio_es: " Dispone de sistema de evacuación")</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>179</v>
+      </c>
+      <c r="B291" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C291" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D291" t="s">
+        <v>1718</v>
+      </c>
+      <c r="F291" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "fosa_septica", sistema_element: "sanejament", descripcio_ca: "Disposa de sistema d'evacuació propi (fossa sèptica, etc.)", descripcio_es: " Dispone de sistema de evacuación propio (fosa séptica, etc.)")</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>179</v>
+      </c>
+      <c r="B292" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C292" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D292" t="s">
+        <v>1719</v>
+      </c>
+      <c r="F292" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_vistos", sistema_element: "sanejament", descripcio_ca: "Els col·lectors són vistos", descripcio_es: " Los colectors son vistos")</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>179</v>
+      </c>
+      <c r="B293" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C293" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D293" t="s">
+        <v>1720</v>
+      </c>
+      <c r="F293" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "bomba_elevacio", sistema_element: "sanejament", descripcio_ca: "Disposa de bomba d'elevació", descripcio_es: " Dispone de bomba de elevación")</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>179</v>
+      </c>
+      <c r="B294" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C294" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D294" t="s">
+        <v>1721</v>
+      </c>
+      <c r="F294" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "separador_greixos", sistema_element: "sanejament", descripcio_ca: "Disposa de separador de greixos i fangs", descripcio_es: " Dispone de separador de grasas y barros")</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>179</v>
+      </c>
+      <c r="B295" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C295" t="s">
+        <v>1688</v>
+      </c>
+      <c r="D295" t="s">
+        <v>1722</v>
+      </c>
+      <c r="F295" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_vistos", sistema_element: "sanejament", descripcio_ca: "Baixants vistos", descripcio_es: " Bajantes vistos")</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>179</v>
+      </c>
+      <c r="B296" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C296" t="s">
+        <v>1690</v>
+      </c>
+      <c r="D296" t="s">
+        <v>1723</v>
+      </c>
+      <c r="F296" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_encastats", sistema_element: "sanejament", descripcio_ca: "Baixants encastats", descripcio_es: " Bajantes encastados")</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>179</v>
+      </c>
+      <c r="B297" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C297" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D297" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F297" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_ceramics", sistema_element: "sanejament", descripcio_ca: "Baixants ceràmics", descripcio_es: " Bajantes cerámicos")</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>179</v>
+      </c>
+      <c r="B298" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C298" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D298" t="s">
+        <v>1725</v>
+      </c>
+      <c r="F298" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_pvc", sistema_element: "sanejament", descripcio_ca: "Baixants de PVC", descripcio_es: " Bajantes de PVC")</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>179</v>
+      </c>
+      <c r="B299" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C299" t="s">
+        <v>1696</v>
+      </c>
+      <c r="D299" t="s">
+        <v>1726</v>
+      </c>
+      <c r="F299" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_fibrociment", sistema_element: "sanejament", descripcio_ca: "Baixants de fibrociment", descripcio_es: " Bajantes de fibrocemento")</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>179</v>
+      </c>
+      <c r="B300" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1698</v>
+      </c>
+      <c r="D300" t="s">
+        <v>1727</v>
+      </c>
+      <c r="F300" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_coure", sistema_element: "sanejament", descripcio_ca: "Baixants de coure", descripcio_es: " Bajantes de cobre")</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>179</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1700</v>
+      </c>
+      <c r="D301" t="s">
+        <v>1728</v>
+      </c>
+      <c r="F301" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_alumini", sistema_element: "sanejament", descripcio_ca: "Baixants d'alumini", descripcio_es: " Bajantes de aluminio")</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>179</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1702</v>
+      </c>
+      <c r="D302" t="s">
+        <v>1729</v>
+      </c>
+      <c r="F302" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_polipropile", sistema_element: "sanejament", descripcio_ca: "Baixants de polipropilè", descripcio_es: " Bajantes de polipropileno")</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>179</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1704</v>
+      </c>
+      <c r="D303" t="s">
+        <v>1730</v>
+      </c>
+      <c r="F303" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "baixants_zinc", sistema_element: "sanejament", descripcio_ca: "Baixants de zinc", descripcio_es: " Bajantes de zinc")</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>179</v>
+      </c>
+      <c r="B304" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D304" t="s">
+        <v>1731</v>
+      </c>
+      <c r="F304" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_vistos", sistema_element: "sanejament", descripcio_ca: "Col·lectors vistos", descripcio_es: " Colectores vistos")</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>179</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1706</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D305" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F305" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_soterrats", sistema_element: "sanejament", descripcio_ca: "Col·lectors soterrats", descripcio_es: " Colectores enterrados")</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>179</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1708</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D306" t="s">
+        <v>1733</v>
+      </c>
+      <c r="F306" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_formigo", sistema_element: "sanejament", descripcio_ca: "Col·lectors de formigó", descripcio_es: " Colectores de hormigón")</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>179</v>
+      </c>
+      <c r="B307" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C307" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D307" t="s">
+        <v>1734</v>
+      </c>
+      <c r="F307" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_ceramic", sistema_element: "sanejament", descripcio_ca: "Col·lectors ceràmics", descripcio_es: " Colectores cerámicos")</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>179</v>
+      </c>
+      <c r="B308" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D308" t="s">
+        <v>1735</v>
+      </c>
+      <c r="F308" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_fibrociment", sistema_element: "sanejament", descripcio_ca: "Col·lectors de fibrociment", descripcio_es: " Colectores de fibrocemento")</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>179</v>
+      </c>
+      <c r="B309" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C309" t="s">
+        <v>1715</v>
+      </c>
+      <c r="D309" t="s">
+        <v>1736</v>
+      </c>
+      <c r="F309" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "colectors_pvc", sistema_element: "sanejament", descripcio_ca: "Col·lectors de PVC", descripcio_es: " Colectores de PVC")</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>121</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D310" t="s">
+        <v>1738</v>
+      </c>
+      <c r="F310" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "connexio_directa", sistema_element: "aigua", descripcio_ca: "Disposa de connexió directa a xarxa pública de subministrament d'aigua", descripcio_es: "Dispone de conexión directa a red pública de suministro de agua")</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>121</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1756</v>
+      </c>
+      <c r="D311" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F311" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "connexio_aforament", sistema_element: "aigua", descripcio_ca: "Disposa de connexió per aforament a xarxa pública de subministrament d'aigua", descripcio_es: "Dispone de conexión por aforo a red pública de suministro de agua")</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>121</v>
+      </c>
+      <c r="B312" t="s">
+        <v>1741</v>
+      </c>
+      <c r="C312" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D312" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F312" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "captacio_propia", sistema_element: "aigua", descripcio_ca: "Disposa de captació pròpia (pou, bomba, etc.)", descripcio_es: "Dispone de captación propia (pozo, bomba, etc.)")</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>121</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1743</v>
+      </c>
+      <c r="C313" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D313" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F313" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "grup_pressio", sistema_element: "aigua", descripcio_ca: "Disposa de grup de pressió", descripcio_es: "Dispone de grupo de presión")</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>121</v>
+      </c>
+      <c r="B314" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1759</v>
+      </c>
+      <c r="D314" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F314" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptador_unic", sistema_element: "aigua", descripcio_ca: "Comptador únic per tot l'edifici", descripcio_es: "Contador único para todo el edificio")</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>121</v>
+      </c>
+      <c r="B315" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D315" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F315" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptadors_individuals_habitatge", sistema_element: "aigua", descripcio_ca: "Comptadors individuals per habitatge/local", descripcio_es: "Contadores individuales por vivienda/local")</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>121</v>
+      </c>
+      <c r="B316" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C316" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D316" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F316" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptadors_individuals_centralitzats", sistema_element: "aigua", descripcio_ca: "Comptadors individuals centralitzats", descripcio_es: "Contadores individuales centralizados")</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>121</v>
+      </c>
+      <c r="B317" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C317" t="s">
+        <v>1762</v>
+      </c>
+      <c r="D317" t="s">
+        <v>1766</v>
+      </c>
+      <c r="F317" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "muntants_plom", sistema_element: "aigua", descripcio_ca: "Muntants de plom", descripcio_es: "Montantes de plomo")</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>121</v>
+      </c>
+      <c r="B318" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C318" t="s">
+        <v>1763</v>
+      </c>
+      <c r="D318" t="s">
+        <v>1767</v>
+      </c>
+      <c r="F318" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "muntants_ferro", sistema_element: "aigua", descripcio_ca: "Muntants de ferro", descripcio_es: "Montantes de hierro")</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>121</v>
+      </c>
+      <c r="B319" t="s">
+        <v>1753</v>
+      </c>
+      <c r="C319" t="s">
+        <v>1764</v>
+      </c>
+      <c r="D319" t="s">
+        <v>1768</v>
+      </c>
+      <c r="F319" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "muntants_coure", sistema_element: "aigua", descripcio_ca: "Muntants de coure", descripcio_es: "Montantes de cobre")</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>121</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C320" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D320" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F320" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "muntants_plastic", sistema_element: "aigua", descripcio_ca: "Muntants de plàstic", descripcio_es: "Montantes de plástico")</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>125</v>
+      </c>
+      <c r="B321" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C321" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D321" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F321" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "enllumenat_comunitari", sistema_element: "electricitat", descripcio_ca: "Disposa d'enllumenat comunitari", descripcio_es: "Dispone de alumbrado comunitario")</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>125</v>
+      </c>
+      <c r="B322" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C322" t="s">
+        <v>1781</v>
+      </c>
+      <c r="D322" t="s">
+        <v>1773</v>
+      </c>
+      <c r="F322" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "mes_100k", sistema_element: "electricitat", descripcio_ca: "Potència total instal·lada superior als 100 kW", descripcio_es: "Potencia total instalada superior a los 100 kW")</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>125</v>
+      </c>
+      <c r="B323" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C323" t="s">
+        <v>1782</v>
+      </c>
+      <c r="D323" t="s">
+        <v>1775</v>
+      </c>
+      <c r="F323" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "connexio_terra", sistema_element: "electricitat", descripcio_ca: "Disposa de connexió a terra", descripcio_es: "Dispone de conexión a tierra")</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>125</v>
+      </c>
+      <c r="B324" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C324" t="s">
+        <v>1783</v>
+      </c>
+      <c r="D324" t="s">
+        <v>1777</v>
+      </c>
+      <c r="F324" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "centre_transformacio", sistema_element: "electricitat", descripcio_ca: "Hi ha un centre de transformació a l'edifici", descripcio_es: "Hay un centro de transformación en el edificio")</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>125</v>
+      </c>
+      <c r="B325" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C325" t="s">
+        <v>1784</v>
+      </c>
+      <c r="D325" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F325" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "fotovoltaica", sistema_element: "electricitat", descripcio_ca: "Disposa d'instal·lació solar fotovoltaica", descripcio_es: "Dispone de instalación solar fotovoltaica")</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>125</v>
+      </c>
+      <c r="B326" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C326" t="s">
+        <v>1759</v>
+      </c>
+      <c r="D326" t="s">
+        <v>1746</v>
+      </c>
+      <c r="F326" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptador_unic", sistema_element: "electricitat", descripcio_ca: "Comptador únic per tot l'edifici", descripcio_es: "Contador único para todo el edificio")</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>125</v>
+      </c>
+      <c r="B327" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C327" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D327" t="s">
+        <v>1748</v>
+      </c>
+      <c r="F327" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptadors_individuals_habitatge", sistema_element: "electricitat", descripcio_ca: "Comptadors individuals per habitatge/local", descripcio_es: "Contadores individuales por vivienda/local")</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>125</v>
+      </c>
+      <c r="B328" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C328" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D328" t="s">
+        <v>1750</v>
+      </c>
+      <c r="F328" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "comptadors_individuals_centralitzats", sistema_element: "electricitat", descripcio_ca: "Comptadors individuals centralitzats", descripcio_es: "Contadores individuales centralizados")</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>207</v>
+      </c>
+      <c r="B329" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C329" t="s">
+        <v>1809</v>
+      </c>
+      <c r="D329" t="s">
+        <v>1812</v>
+      </c>
+      <c r="F329" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "escalfador_pn_menor_24", sistema_element: "climatitzacio", descripcio_ca: "Escalfador Pn ≤ 24,4 kW", descripcio_es: "Calentador Pn ≤ 24,4 kW")</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>207</v>
+      </c>
+      <c r="B330" t="s">
+        <v>1786</v>
+      </c>
+      <c r="C330" t="s">
+        <v>1810</v>
+      </c>
+      <c r="D330" t="s">
+        <v>1813</v>
+      </c>
+      <c r="F330" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "escalfador_pn_24_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador 24,4 kW &lt; Pn ≤ 70 kW", descripcio_es: "Calentador 24,4 kW &lt; Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>207</v>
+      </c>
+      <c r="B331" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C331" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F331" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "escalfador_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador Pn &gt; 70 kW", descripcio_es: "Calentador Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>207</v>
+      </c>
+      <c r="B332" t="s">
+        <v>1788</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1789</v>
+      </c>
+      <c r="D332" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F332" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "caldera_gas_pn_menor_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera a gas Pn ≤ 70 kW", descripcio_es: "Caldera a gas Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>207</v>
+      </c>
+      <c r="B333" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1791</v>
+      </c>
+      <c r="D333" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F333" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "caldera_gas_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera a gas Pn &gt; 70 kW", descripcio_es: "Caldera a gas Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>207</v>
+      </c>
+      <c r="B334" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D334" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F334" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "caldera_biomassa", sistema_element: "climatitzacio", descripcio_ca: "Caldera a biomassa", descripcio_es: "Caldera a biomasa")</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>207</v>
+      </c>
+      <c r="B335" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1808</v>
+      </c>
+      <c r="D335" t="s">
+        <v>1795</v>
+      </c>
+      <c r="F335" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "caldera_solar_termica", sistema_element: "climatitzacio", descripcio_ca: "Caldera o escalfador amb instal·lació d’energia solar tèrmica", descripcio_es: "Caldera o calentador con instalación de energía solar térmica")</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>207</v>
+      </c>
+      <c r="B336" t="s">
+        <v>1796</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1815</v>
+      </c>
+      <c r="F336" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "altres_pn_menor_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera Pn ≤ 70 kW", descripcio_es: "Caldera Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>207</v>
+      </c>
+      <c r="B337" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1816</v>
+      </c>
+      <c r="D337" t="s">
+        <v>1816</v>
+      </c>
+      <c r="F337" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "altres_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera Pn &gt; 70 kW", descripcio_es: "Caldera Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>207</v>
+      </c>
+      <c r="B338" t="s">
+        <v>1798</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1817</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1819</v>
+      </c>
+      <c r="F338" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_menor_12_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom Pn ≤ 12 kW", descripcio_es: "Sistema de climatización autónomo Pn ≤ 12 kW")</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>207</v>
+      </c>
+      <c r="B339" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1818</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1820</v>
+      </c>
+      <c r="F339" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_menor_12_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració Pn ≤ 12 kW", descripcio_es: "Sistema de climatización con torre de refrigeración Pn ≤ 12 kW ")</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>207</v>
+      </c>
+      <c r="B340" t="s">
+        <v>1800</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1826</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1821</v>
+      </c>
+      <c r="F340" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_menor_12_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor Pn ≤ 12 kW", descripcio_es: "Sistema de climatización con recuperación de calor Pn ≤ 12 kW")</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
+        <v>207</v>
+      </c>
+      <c r="B341" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C341" t="s">
+        <v>1822</v>
+      </c>
+      <c r="D341" t="s">
+        <v>1829</v>
+      </c>
+      <c r="F341" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización autónomo 12 kW &lt; Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A342" t="s">
+        <v>207</v>
+      </c>
+      <c r="B342" t="s">
+        <v>1802</v>
+      </c>
+      <c r="C342" t="s">
+        <v>1824</v>
+      </c>
+      <c r="D342" t="s">
+        <v>1830</v>
+      </c>
+      <c r="F342" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración 12 kW &lt; Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A343" t="s">
+        <v>207</v>
+      </c>
+      <c r="B343" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1827</v>
+      </c>
+      <c r="D343" t="s">
+        <v>1833</v>
+      </c>
+      <c r="F343" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor 12 kW &lt; Pn ≤ 70 kW")</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A344" t="s">
+        <v>207</v>
+      </c>
+      <c r="B344" t="s">
+        <v>1804</v>
+      </c>
+      <c r="C344" t="s">
+        <v>1823</v>
+      </c>
+      <c r="D344" t="s">
+        <v>1832</v>
+      </c>
+      <c r="F344" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom Pn &gt; 70 kW", descripcio_es: "Sistema de climatización autónomo Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A345" t="s">
+        <v>207</v>
+      </c>
+      <c r="B345" t="s">
+        <v>1805</v>
+      </c>
+      <c r="C345" t="s">
+        <v>1825</v>
+      </c>
+      <c r="D345" t="s">
+        <v>1831</v>
+      </c>
+      <c r="F345" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració Pn &gt; 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A346" t="s">
+        <v>207</v>
+      </c>
+      <c r="B346" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C346" t="s">
+        <v>1828</v>
+      </c>
+      <c r="D346" t="s">
+        <v>1834</v>
+      </c>
+      <c r="F346" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor Pn &gt; 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor Pn &gt; 70 kW")</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A347" t="s">
+        <v>162</v>
+      </c>
+      <c r="B347" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D347" t="s">
+        <v>1836</v>
+      </c>
+      <c r="F347" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "instalacio_gas", sistema_element: "gas", descripcio_ca: "Escomesa a xarxa de distribució canalitzada de gas per a ús domèstic", descripcio_es: "Acometida a red de distribución canalizada de gas para uso doméstico")</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A348" t="s">
+        <v>162</v>
+      </c>
+      <c r="B348" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C348" t="s">
+        <v>1842</v>
+      </c>
+      <c r="D348" t="s">
+        <v>1839</v>
+      </c>
+      <c r="F348" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "diposit_aire_lliure", sistema_element: "gas", descripcio_ca: "Dipòsit de gas propà a l'aire lliure", descripcio_es: "Depósito de gas propano al aire libre")</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A349" t="s">
+        <v>162</v>
+      </c>
+      <c r="B349" t="s">
+        <v>1838</v>
+      </c>
+      <c r="C349" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D349" t="s">
+        <v>1840</v>
+      </c>
+      <c r="F349" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "diposit_enterrat", sistema_element: "gas", descripcio_ca: "Dipòsit de gas propà enterrat", descripcio_es: "Depósito de gas propano enterrado")</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A350" t="s">
+        <v>396</v>
+      </c>
+      <c r="B350" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C350" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D350" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F350" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "habitatge_natural_conductes", sistema_element: "ventilacio", descripcio_ca: "Natural per conductes", descripcio_es: "Natural por conductos")</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A351" t="s">
+        <v>396</v>
+      </c>
+      <c r="B351" t="s">
+        <v>1846</v>
+      </c>
+      <c r="C351" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D351" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F351" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "habitatge_natural_obertures", sistema_element: "ventilacio", descripcio_ca: "Natural per obertures", descripcio_es: "Natural por aperturas")</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A352" t="s">
+        <v>396</v>
+      </c>
+      <c r="B352" t="s">
+        <v>1848</v>
+      </c>
+      <c r="C352" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D352" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F352" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "habitatge_mecanica_conductes", sistema_element: "ventilacio", descripcio_ca: "Mecànica per conductes", descripcio_es: "Mecánica por conductos")</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A353" t="s">
+        <v>396</v>
+      </c>
+      <c r="B353" t="s">
+        <v>1850</v>
+      </c>
+      <c r="C353" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D353" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F353" t="str">
+        <f t="shared" si="4"/>
+        <v>ElementPredefinit.create(nom_element: "habitatge_mecanica_obertures", sistema_element: "ventilacio", descripcio_ca: "Mecànica per obertures", descripcio_es: "Mecánica por aperturas")</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>396</v>
+      </c>
+      <c r="B354" t="s">
+        <v>1852</v>
+      </c>
+      <c r="C354" t="s">
+        <v>1873</v>
+      </c>
+      <c r="D354" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F354" t="str">
+        <f t="shared" ref="F354:F404" si="5">"ElementPredefinit.create(nom_element: """&amp;B354&amp;""", sistema_element: """&amp;A354&amp;""", descripcio_ca: """&amp;C354&amp;""", descripcio_es: """&amp;D354&amp;""")"</f>
+        <v>ElementPredefinit.create(nom_element: "habitatge_mecanica_control", sistema_element: "ventilacio", descripcio_ca: "Mecànica amb sistema de control", descripcio_es: "Mecánica con sistema de control")</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A355" t="s">
+        <v>396</v>
+      </c>
+      <c r="B355" t="s">
+        <v>1854</v>
+      </c>
+      <c r="C355" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D355" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F355" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "traster_natural_conductes", sistema_element: "ventilacio", descripcio_ca: "Natural per conductes", descripcio_es: "Natural por conductos")</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A356" t="s">
+        <v>396</v>
+      </c>
+      <c r="B356" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C356" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D356" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F356" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "traster_natural_obertures", sistema_element: "ventilacio", descripcio_ca: "Natural per obertures", descripcio_es: "Natural por aperturas")</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A357" t="s">
+        <v>396</v>
+      </c>
+      <c r="B357" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C357" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D357" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F357" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "traster_mecanica_conductes", sistema_element: "ventilacio", descripcio_ca: "Mecànica per conductes", descripcio_es: "Mecánica por conductos")</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A358" t="s">
+        <v>396</v>
+      </c>
+      <c r="B358" t="s">
+        <v>1857</v>
+      </c>
+      <c r="C358" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D358" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F358" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "traster_mecanica_obertures", sistema_element: "ventilacio", descripcio_ca: "Mecànica per obertures", descripcio_es: "Mecánica por aperturas")</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A359" t="s">
+        <v>396</v>
+      </c>
+      <c r="B359" t="s">
+        <v>1858</v>
+      </c>
+      <c r="C359" t="s">
+        <v>1873</v>
+      </c>
+      <c r="D359" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F359" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "traster_mecanica_control", sistema_element: "ventilacio", descripcio_ca: "Mecànica amb sistema de control", descripcio_es: "Mecánica con sistema de control")</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A360" t="s">
+        <v>396</v>
+      </c>
+      <c r="B360" t="s">
+        <v>1859</v>
+      </c>
+      <c r="C360" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D360" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F360" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "magatzem_natural_conductes", sistema_element: "ventilacio", descripcio_ca: "Natural per conductes", descripcio_es: "Natural por conductos")</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A361" t="s">
+        <v>396</v>
+      </c>
+      <c r="B361" t="s">
+        <v>1860</v>
+      </c>
+      <c r="C361" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D361" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F361" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "magatzem_natural_obertures", sistema_element: "ventilacio", descripcio_ca: "Natural per obertures", descripcio_es: "Natural por aperturas")</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A362" t="s">
+        <v>396</v>
+      </c>
+      <c r="B362" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C362" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D362" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F362" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "magatzem_mecanica_conductes", sistema_element: "ventilacio", descripcio_ca: "Mecànica per conductes", descripcio_es: "Mecánica por conductos")</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A363" t="s">
+        <v>396</v>
+      </c>
+      <c r="B363" t="s">
+        <v>1862</v>
+      </c>
+      <c r="C363" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D363" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F363" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "magatzem_mecanica_obertures", sistema_element: "ventilacio", descripcio_ca: "Mecànica per obertures", descripcio_es: "Mecánica por aperturas")</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A364" t="s">
+        <v>396</v>
+      </c>
+      <c r="B364" t="s">
+        <v>1863</v>
+      </c>
+      <c r="C364" t="s">
+        <v>1873</v>
+      </c>
+      <c r="D364" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F364" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "magatzem_mecanica_control", sistema_element: "ventilacio", descripcio_ca: "Mecànica amb sistema de control", descripcio_es: "Mecánica con sistema de control")</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A365" t="s">
+        <v>396</v>
+      </c>
+      <c r="B365" t="s">
+        <v>1864</v>
+      </c>
+      <c r="C365" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D365" t="s">
+        <v>1845</v>
+      </c>
+      <c r="F365" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "garatge_natural_conductes", sistema_element: "ventilacio", descripcio_ca: "Natural per conductes", descripcio_es: "Natural por conductos")</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A366" t="s">
+        <v>396</v>
+      </c>
+      <c r="B366" t="s">
+        <v>1865</v>
+      </c>
+      <c r="C366" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D366" t="s">
+        <v>1847</v>
+      </c>
+      <c r="F366" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "garatge_natural_obertures", sistema_element: "ventilacio", descripcio_ca: "Natural per obertures", descripcio_es: "Natural por aperturas")</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A367" t="s">
+        <v>396</v>
+      </c>
+      <c r="B367" t="s">
+        <v>1866</v>
+      </c>
+      <c r="C367" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D367" t="s">
+        <v>1849</v>
+      </c>
+      <c r="F367" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "garatge_mecanica_conductes", sistema_element: "ventilacio", descripcio_ca: "Mecànica per conductes", descripcio_es: "Mecánica por conductos")</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A368" t="s">
+        <v>396</v>
+      </c>
+      <c r="B368" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C368" t="s">
+        <v>1872</v>
+      </c>
+      <c r="D368" t="s">
+        <v>1851</v>
+      </c>
+      <c r="F368" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "garatge_mecanica_obertures", sistema_element: "ventilacio", descripcio_ca: "Mecànica per obertures", descripcio_es: "Mecánica por aperturas")</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A369" t="s">
+        <v>396</v>
+      </c>
+      <c r="B369" t="s">
+        <v>1868</v>
+      </c>
+      <c r="C369" t="s">
+        <v>1873</v>
+      </c>
+      <c r="D369" t="s">
+        <v>1853</v>
+      </c>
+      <c r="F369" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "garatge_mecanica_control", sistema_element: "ventilacio", descripcio_ca: "Mecànica amb sistema de control", descripcio_es: "Mecánica con sistema de control")</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A370" t="s">
+        <v>462</v>
+      </c>
+      <c r="B370" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C370" t="s">
+        <v>1892</v>
+      </c>
+      <c r="D370" t="s">
+        <v>1875</v>
+      </c>
+      <c r="F370" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "alarma_automatica", sistema_element: "incendis", descripcio_ca: "Sistema automàtic de detecció i alarma d’incendis", descripcio_es: "Sistema automático de detección y alarma de incendios")</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A371" t="s">
+        <v>462</v>
+      </c>
+      <c r="B371" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C371" t="s">
+        <v>1893</v>
+      </c>
+      <c r="D371" t="s">
+        <v>1877</v>
+      </c>
+      <c r="F371" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "alarma_manual", sistema_element: "incendis", descripcio_ca: "Sistema manual d’alarma d’incendis", descripcio_es: "Sistema manual de alarma de incendios")</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A372" t="s">
+        <v>462</v>
+      </c>
+      <c r="B372" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C372" t="s">
+        <v>1894</v>
+      </c>
+      <c r="D372" t="s">
+        <v>1879</v>
+      </c>
+      <c r="F372" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "extintors", sistema_element: "incendis", descripcio_ca: "Extintors d’incendis", descripcio_es: "Extintores de incendios")</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A373" t="s">
+        <v>462</v>
+      </c>
+      <c r="B373" t="s">
+        <v>1880</v>
+      </c>
+      <c r="C373" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D373" t="s">
+        <v>1881</v>
+      </c>
+      <c r="F373" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "abastiment_aigua", sistema_element: "incendis", descripcio_ca: "Sistema d’abastiment d’aigua contra incendis", descripcio_es: "Sistema de suministro de agua contra incendios")</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A374" t="s">
+        <v>462</v>
+      </c>
+      <c r="B374" t="s">
+        <v>1882</v>
+      </c>
+      <c r="C374" t="s">
+        <v>1896</v>
+      </c>
+      <c r="D374" t="s">
+        <v>1883</v>
+      </c>
+      <c r="F374" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "bie", sistema_element: "incendis", descripcio_ca: "Boca d’incendis equipada (BIE)", descripcio_es: "Boca de incendios equipada (BIE)")</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A375" t="s">
+        <v>462</v>
+      </c>
+      <c r="B375" t="s">
+        <v>1884</v>
+      </c>
+      <c r="C375" t="s">
+        <v>1897</v>
+      </c>
+      <c r="D375" t="s">
+        <v>1885</v>
+      </c>
+      <c r="F375" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "hidrants", sistema_element: "incendis", descripcio_ca: "Hidrants", descripcio_es: "Hidrantes")</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A376" t="s">
+        <v>462</v>
+      </c>
+      <c r="B376" t="s">
+        <v>1886</v>
+      </c>
+      <c r="C376" t="s">
+        <v>1898</v>
+      </c>
+      <c r="D376" t="s">
+        <v>1887</v>
+      </c>
+      <c r="F376" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "ruixadors", sistema_element: "incendis", descripcio_ca: "Sistemes fixes d’extinció (ruixadors)", descripcio_es: "Sistema fijo de extinción (rociadores)")</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A377" t="s">
+        <v>462</v>
+      </c>
+      <c r="B377" t="s">
+        <v>1888</v>
+      </c>
+      <c r="C377" t="s">
+        <v>1899</v>
+      </c>
+      <c r="D377" t="s">
+        <v>1889</v>
+      </c>
+      <c r="F377" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "columnes_seques", sistema_element: "incendis", descripcio_ca: "Columnes seques", descripcio_es: "Columnas secas")</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A378" t="s">
+        <v>462</v>
+      </c>
+      <c r="B378" t="s">
+        <v>1890</v>
+      </c>
+      <c r="C378" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D378" t="s">
+        <v>1891</v>
+      </c>
+      <c r="F378" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "parallamps", sistema_element: "incendis", descripcio_ca: "Parallamps", descripcio_es: "Pararayos")</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A379" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B379" t="s">
+        <v>1901</v>
+      </c>
+      <c r="C379" t="s">
+        <v>1911</v>
+      </c>
+      <c r="D379" t="s">
+        <v>1906</v>
+      </c>
+      <c r="F379" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "habitatge_unifamiliar", sistema_element: "ascensors", descripcio_ca: "L'habitatge disposa d'ascensor", descripcio_es: "La vivienda dispone de ascensor")</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A380" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B380" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C380" t="s">
+        <v>1909</v>
+      </c>
+      <c r="D380" t="s">
+        <v>1903</v>
+      </c>
+      <c r="F380" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "edifici_comunitari", sistema_element: "ascensors", descripcio_ca: "Ascensor en edifici comunitari d’ús residencial de fins a sis parades, amb antiguitat menor de 20 anys", descripcio_es: "Ascensor en edificio comunitario de uso residencial de hasta seis paradas, con antigüedad menor de 20 años")</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A381" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B381" t="s">
+        <v>1904</v>
+      </c>
+      <c r="C381" t="s">
+        <v>1910</v>
+      </c>
+      <c r="D381" t="s">
+        <v>1907</v>
+      </c>
+      <c r="F381" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "mes_20_plantes", sistema_element: "ascensors", descripcio_ca: "Ascensor instal·lat en edifici de més de 20 habitatges, o amb més de 4 plantes servides", descripcio_es: "Ascensor instalado en edificios de más de 20 viviendas, o con más de 4 plantas servidas")</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A382" t="s">
+        <v>1912</v>
+      </c>
+      <c r="B382" t="s">
+        <v>1905</v>
+      </c>
+      <c r="C382" t="s">
+        <v>1908</v>
+      </c>
+      <c r="D382" t="s">
+        <v>1908</v>
+      </c>
+      <c r="F382" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "altres", sistema_element: "ascensors", descripcio_ca: "Ascensor", descripcio_es: "Ascensor")</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A383" t="s">
+        <v>600</v>
+      </c>
+      <c r="B383" t="s">
+        <v>1913</v>
+      </c>
+      <c r="C383" t="s">
+        <v>1935</v>
+      </c>
+      <c r="D383" t="s">
+        <v>1914</v>
+      </c>
+      <c r="F383" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "porter_audio", sistema_element: "telecomunicacions", descripcio_ca: "Porter electrònic amb sistema d'àudio", descripcio_es: "Portero electrónico con sistema de audio")</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A384" t="s">
+        <v>600</v>
+      </c>
+      <c r="B384" t="s">
+        <v>1915</v>
+      </c>
+      <c r="C384" t="s">
+        <v>1936</v>
+      </c>
+      <c r="D384" t="s">
+        <v>1916</v>
+      </c>
+      <c r="F384" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "porter_video", sistema_element: "telecomunicacions", descripcio_ca: "Porter electrònic amb sistema d'àudio i vídeo", descripcio_es: "Portero electrónico con sistema de audio y vídeo")</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A385" t="s">
+        <v>600</v>
+      </c>
+      <c r="B385" t="s">
+        <v>1917</v>
+      </c>
+      <c r="C385" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D385" t="s">
+        <v>1918</v>
+      </c>
+      <c r="F385" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "antena_individual", sistema_element: "telecomunicacions", descripcio_ca: "Antena individual i xarxa coaxial", descripcio_es: "Antena individual y red coaxial")</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A386" t="s">
+        <v>600</v>
+      </c>
+      <c r="B386" t="s">
+        <v>1919</v>
+      </c>
+      <c r="C386" t="s">
+        <v>1938</v>
+      </c>
+      <c r="D386" t="s">
+        <v>1920</v>
+      </c>
+      <c r="F386" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "antena_colectiva", sistema_element: "telecomunicacions", descripcio_ca: "Antena col·lectiva i xarxa coaxial", descripcio_es: "Antena colectiva y red coaxial")</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A387" t="s">
+        <v>600</v>
+      </c>
+      <c r="B387" t="s">
+        <v>1921</v>
+      </c>
+      <c r="C387" t="s">
+        <v>1939</v>
+      </c>
+      <c r="D387" t="s">
+        <v>1922</v>
+      </c>
+      <c r="F387" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "parabolica_individual", sistema_element: "telecomunicacions", descripcio_ca: "Antena parabòlica individual", descripcio_es: "Antena parabólica individual")</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A388" t="s">
+        <v>600</v>
+      </c>
+      <c r="B388" t="s">
+        <v>1923</v>
+      </c>
+      <c r="C388" t="s">
+        <v>1940</v>
+      </c>
+      <c r="D388" t="s">
+        <v>1924</v>
+      </c>
+      <c r="F388" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "parabolica_colectiva", sistema_element: "telecomunicacions", descripcio_ca: "Antena parabòlica col·lectiva", descripcio_es: "Antena parabólica colectiva")</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A389" t="s">
+        <v>600</v>
+      </c>
+      <c r="B389" t="s">
+        <v>1925</v>
+      </c>
+      <c r="C389" t="s">
+        <v>1941</v>
+      </c>
+      <c r="D389" t="s">
+        <v>1926</v>
+      </c>
+      <c r="F389" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "telefonia", sistema_element: "telecomunicacions", descripcio_ca: "Instal·lació de telefonia", descripcio_es: "Instalación de telefonía")</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A390" t="s">
+        <v>600</v>
+      </c>
+      <c r="B390" t="s">
+        <v>1927</v>
+      </c>
+      <c r="C390" t="s">
+        <v>1942</v>
+      </c>
+      <c r="D390" t="s">
+        <v>1928</v>
+      </c>
+      <c r="F390" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "riti", sistema_element: "telecomunicacions", descripcio_ca: "RITI (Recinte d’instal·lacions de telecomunicacions inferior)", descripcio_es: "RITI (Recinto de instalaciones de telecomunicaciones inferior)")</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A391" t="s">
+        <v>600</v>
+      </c>
+      <c r="B391" t="s">
+        <v>1929</v>
+      </c>
+      <c r="C391" t="s">
+        <v>1943</v>
+      </c>
+      <c r="D391" t="s">
+        <v>1930</v>
+      </c>
+      <c r="F391" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "rits", sistema_element: "telecomunicacions", descripcio_ca: "RITS (Recinte d’instal·lacions de telecomunicacions superior)", descripcio_es: "RITS (Recinto de instalaciones de telecomunicaciones superior)")</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A392" t="s">
+        <v>600</v>
+      </c>
+      <c r="B392" t="s">
+        <v>1931</v>
+      </c>
+      <c r="C392" t="s">
+        <v>1944</v>
+      </c>
+      <c r="D392" t="s">
+        <v>1932</v>
+      </c>
+      <c r="F392" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "ritu", sistema_element: "telecomunicacions", descripcio_ca: "RITU (Recinte d’instal·lacions de telecomunicacions únic)", descripcio_es: "RITU (Recinto de instalaciones de telecomunicaciones único)")</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A393" t="s">
+        <v>600</v>
+      </c>
+      <c r="B393" t="s">
+        <v>1933</v>
+      </c>
+      <c r="C393" t="s">
+        <v>1945</v>
+      </c>
+      <c r="D393" t="s">
+        <v>1934</v>
+      </c>
+      <c r="F393" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "ritm", sistema_element: "telecomunicacions", descripcio_ca: "RITM (Recinte d’instal·lacions de telecomunicacions únic modular prefabricat)", descripcio_es: "RITM (Recinto de instalaciones de telecomunicaciones único modular prefabricado)")</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A394" t="s">
+        <v>633</v>
+      </c>
+      <c r="B394" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C394" t="s">
+        <v>1973</v>
+      </c>
+      <c r="D394" t="s">
+        <v>1976</v>
+      </c>
+      <c r="F394" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_estructura_obra", sistema_element: "especials", descripcio_ca: "Piscina amb estructura d'obra", descripcio_es: "Piscina con estructura de obra")</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A395" t="s">
+        <v>633</v>
+      </c>
+      <c r="B395" t="s">
+        <v>1947</v>
+      </c>
+      <c r="C395" t="s">
+        <v>1974</v>
+      </c>
+      <c r="D395" t="s">
+        <v>1977</v>
+      </c>
+      <c r="F395" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_estructura_composite", sistema_element: "especials", descripcio_ca: "Piscina amb estructura de materials composites", descripcio_es: "Piscina con estructura de materiales composites")</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A396" t="s">
+        <v>633</v>
+      </c>
+      <c r="B396" t="s">
+        <v>1948</v>
+      </c>
+      <c r="C396" t="s">
+        <v>1975</v>
+      </c>
+      <c r="D396" t="s">
+        <v>1978</v>
+      </c>
+      <c r="F396" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_estructura_acer", sistema_element: "especials", descripcio_ca: "Piscina amb estructura d'acer", descripcio_es: "Piscina con estructura de acero")</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A397" t="s">
+        <v>633</v>
+      </c>
+      <c r="B397" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C397" t="s">
+        <v>1965</v>
+      </c>
+      <c r="D397" t="s">
+        <v>1950</v>
+      </c>
+      <c r="F397" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_vores_formigo", sistema_element: "especials", descripcio_ca: "Vores prefabricades de formigó", descripcio_es: "Bordes prefabricados de hormigón")</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A398" t="s">
+        <v>633</v>
+      </c>
+      <c r="B398" t="s">
+        <v>1951</v>
+      </c>
+      <c r="C398" t="s">
+        <v>1966</v>
+      </c>
+      <c r="D398" t="s">
+        <v>1952</v>
+      </c>
+      <c r="F398" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_vores_pedra", sistema_element: "especials", descripcio_ca: "Vores de pedra natural", descripcio_es: "Bordes de piedra natural")</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A399" t="s">
+        <v>633</v>
+      </c>
+      <c r="B399" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C399" t="s">
+        <v>1967</v>
+      </c>
+      <c r="D399" t="s">
+        <v>1954</v>
+      </c>
+      <c r="F399" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_ceramica", sistema_element: "especials", descripcio_ca: "Revestiment de peces ceràmiques", descripcio_es: "Revestimiento de piezas cerámicas")</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A400" t="s">
+        <v>633</v>
+      </c>
+      <c r="B400" t="s">
+        <v>1955</v>
+      </c>
+      <c r="C400" t="s">
+        <v>1968</v>
+      </c>
+      <c r="D400" t="s">
+        <v>1956</v>
+      </c>
+      <c r="F400" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_resines", sistema_element: "especials", descripcio_ca: "Revestiment de resines sintètiques", descripcio_es: "Revestimiento de resinas sintéticas")</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A401" t="s">
+        <v>633</v>
+      </c>
+      <c r="B401" t="s">
+        <v>1957</v>
+      </c>
+      <c r="C401" t="s">
+        <v>1969</v>
+      </c>
+      <c r="D401" t="s">
+        <v>1958</v>
+      </c>
+      <c r="F401" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_porcellana", sistema_element: "especials", descripcio_ca: "Revestiment de porcellana", descripcio_es: "Revestimiento de porcelana")</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A402" t="s">
+        <v>633</v>
+      </c>
+      <c r="B402" t="s">
+        <v>1959</v>
+      </c>
+      <c r="C402" t="s">
+        <v>1970</v>
+      </c>
+      <c r="D402" t="s">
+        <v>1960</v>
+      </c>
+      <c r="F402" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_climatitzacio", sistema_element: "especials", descripcio_ca: "Disposa d'instal·lació de climatització", descripcio_es: "Dispone de instalación de climatización")</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A403" t="s">
+        <v>633</v>
+      </c>
+      <c r="B403" t="s">
+        <v>1961</v>
+      </c>
+      <c r="C403" t="s">
+        <v>1971</v>
+      </c>
+      <c r="D403" t="s">
+        <v>1962</v>
+      </c>
+      <c r="F403" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_iluminacio", sistema_element: "especials", descripcio_ca: "Disposa d'instal·lació d'il·luminació submergida", descripcio_es: "Dispone de instalación de iluminación sumergida")</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A404" t="s">
+        <v>633</v>
+      </c>
+      <c r="B404" t="s">
+        <v>1963</v>
+      </c>
+      <c r="C404" t="s">
+        <v>1972</v>
+      </c>
+      <c r="D404" t="s">
+        <v>1964</v>
+      </c>
+      <c r="F404" t="str">
+        <f t="shared" si="5"/>
+        <v>ElementPredefinit.create(nom_element: "piscina_purificador", sistema_element: "especials", descripcio_ca: "Disposa d'instal·lació de purificació d'aigües", descripcio_es: "Dispone de instalación de purificación de aguas")</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F406" t="s">
+        <v>1979</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificació de models per relació amb edifici i creació de json per al document word de l'apartat Dades administratives i jurídiques
</commit_message>
<xml_diff>
--- a/lib/documents_treball/operacions_manteniment_v2.xlsx
+++ b/lib/documents_treball/operacions_manteniment_v2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Operacions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="1980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4989" uniqueCount="1979">
   <si>
     <t>sistema</t>
   </si>
@@ -5962,9 +5962,6 @@
   </si>
   <si>
     <t>Piscina con estructura de acero</t>
-  </si>
-  <si>
-    <t>º</t>
   </si>
 </sst>
 </file>
@@ -6375,8 +6372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N419"/>
   <sheetViews>
-    <sheetView topLeftCell="A392" workbookViewId="0">
-      <selection activeCell="B409" sqref="B409:B419"/>
+    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
+      <selection activeCell="B419" sqref="B419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24180,10 +24177,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F406"/>
+  <dimension ref="A1:F404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A383" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F406" sqref="F406"/>
+    <sheetView topLeftCell="A187" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F289" sqref="F289:F404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31462,11 +31459,6 @@
         <v>ElementPredefinit.create(nom_element: "piscina_purificador", sistema_element: "especials", descripcio_ca: "Disposa d'instal·lació de purificació d'aigües", descripcio_es: "Dispone de instalación de purificación de aguas")</v>
       </c>
     </row>
-    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F406" t="s">
-        <v>1979</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Soluciona error en sistemes de climatització amb símbols de més gran o més petit en les descripcions
</commit_message>
<xml_diff>
--- a/lib/documents_treball/operacions_manteniment_v2.xlsx
+++ b/lib/documents_treball/operacions_manteniment_v2.xlsx
@@ -5397,9 +5397,6 @@
     <t>caldera_gas_pn_major_70</t>
   </si>
   <si>
-    <t>Caldera a gas Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>caldera_biomassa</t>
   </si>
   <si>
@@ -5454,27 +5451,12 @@
     <t>Escalfador Pn ≤ 24,4 kW</t>
   </si>
   <si>
-    <t>Escalfador 24,4 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Escalfador Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>Calentador Pn ≤ 24,4 kW</t>
   </si>
   <si>
-    <t>Calentador 24,4 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Calentador Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>Caldera Pn ≤ 70 kW</t>
   </si>
   <si>
-    <t>Caldera Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>Sistema de climatització autònom Pn ≤ 12 kW</t>
   </si>
   <si>
@@ -5490,45 +5472,9 @@
     <t>Sistema de climatización con recuperación de calor Pn ≤ 12 kW</t>
   </si>
   <si>
-    <t>Sistema de climatització autònom 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatització autònom Pn &gt; 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatització amb torre de refrigeració 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatització amb torre de refrigeració Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>Sistema de climatització amb recuperació de calor Pn ≤ 12 kW</t>
   </si>
   <si>
-    <t>Sistema de climatització amb recuperació de calor 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatització amb recuperació de calor Pn &gt; 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización autónomo 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización con torre de refrigeración 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización con torre de refrigeración Pn &gt; 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización autónomo Pn &gt; 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización con recuperación de calor 12 kW &lt; Pn ≤ 70 kW</t>
-  </si>
-  <si>
-    <t>Sistema de climatización con recuperación de calor Pn &gt; 70 kW</t>
-  </si>
-  <si>
     <t>instalacio_gas</t>
   </si>
   <si>
@@ -5965,6 +5911,60 @@
   </si>
   <si>
     <t>escala_biguetes_formigo_armat</t>
+  </si>
+  <si>
+    <t>Escalfador 24,4 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Calentador 24,4 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització autònom 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización autónomo 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb torre de refrigeració 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb recuperació de calor 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con torre de refrigeración 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con recuperación de calor 12 kW &amp;lt; Pn ≤ 70 kW</t>
+  </si>
+  <si>
+    <t>Escalfador Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Calentador Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Caldera a gas Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Caldera Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització autònom Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb torre de refrigeració Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatització amb recuperació de calor Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización autónomo Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con torre de refrigeración Pn &amp;gt; 70 kW</t>
+  </si>
+  <si>
+    <t>Sistema de climatización con recuperación de calor Pn &amp;gt; 70 kW</t>
   </si>
 </sst>
 </file>
@@ -6375,7 +6375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N419"/>
   <sheetViews>
-    <sheetView topLeftCell="A392" workbookViewId="0">
+    <sheetView topLeftCell="A149" workbookViewId="0">
       <selection activeCell="B419" sqref="B419"/>
     </sheetView>
   </sheetViews>
@@ -24182,16 +24182,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D346" sqref="D346"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="37.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" customWidth="1"/>
-    <col min="4" max="4" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="63.83203125" customWidth="1"/>
+    <col min="4" max="4" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -25293,7 +25293,7 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>1979</v>
+        <v>1961</v>
       </c>
       <c r="C62" t="s">
         <v>1218</v>
@@ -30081,7 +30081,7 @@
         <v>125</v>
       </c>
       <c r="B328" t="s">
-        <v>1978</v>
+        <v>1960</v>
       </c>
       <c r="C328" t="s">
         <v>1760</v>
@@ -30102,10 +30102,10 @@
         <v>1784</v>
       </c>
       <c r="C329" t="s">
+        <v>1807</v>
+      </c>
+      <c r="D329" t="s">
         <v>1808</v>
-      </c>
-      <c r="D329" t="s">
-        <v>1811</v>
       </c>
       <c r="F329" t="str">
         <f t="shared" si="4"/>
@@ -30120,14 +30120,14 @@
         <v>1785</v>
       </c>
       <c r="C330" t="s">
-        <v>1809</v>
+        <v>1962</v>
       </c>
       <c r="D330" t="s">
-        <v>1812</v>
+        <v>1963</v>
       </c>
       <c r="F330" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "escalfador_pn_24_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador 24,4 kW &lt; Pn ≤ 70 kW", descripcio_es: "Calentador 24,4 kW &lt; Pn ≤ 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "escalfador_pn_24_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador 24,4 kW &amp;lt; Pn ≤ 70 kW", descripcio_es: "Calentador 24,4 kW &amp;lt; Pn ≤ 70 kW")</v>
       </c>
     </row>
     <row r="331" spans="1:6" x14ac:dyDescent="0.2">
@@ -30138,14 +30138,14 @@
         <v>1786</v>
       </c>
       <c r="C331" t="s">
-        <v>1810</v>
+        <v>1970</v>
       </c>
       <c r="D331" t="s">
-        <v>1813</v>
+        <v>1971</v>
       </c>
       <c r="F331" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "escalfador_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador Pn &gt; 70 kW", descripcio_es: "Calentador Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "escalfador_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Escalfador Pn &amp;gt; 70 kW", descripcio_es: "Calentador Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="332" spans="1:6" x14ac:dyDescent="0.2">
@@ -30174,14 +30174,14 @@
         <v>1789</v>
       </c>
       <c r="C333" t="s">
-        <v>1790</v>
+        <v>1972</v>
       </c>
       <c r="D333" t="s">
-        <v>1790</v>
+        <v>1972</v>
       </c>
       <c r="F333" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "caldera_gas_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera a gas Pn &gt; 70 kW", descripcio_es: "Caldera a gas Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "caldera_gas_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera a gas Pn &amp;gt; 70 kW", descripcio_es: "Caldera a gas Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
@@ -30189,13 +30189,13 @@
         <v>207</v>
       </c>
       <c r="B334" t="s">
+        <v>1790</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1805</v>
+      </c>
+      <c r="D334" t="s">
         <v>1791</v>
-      </c>
-      <c r="C334" t="s">
-        <v>1806</v>
-      </c>
-      <c r="D334" t="s">
-        <v>1792</v>
       </c>
       <c r="F334" t="str">
         <f t="shared" si="4"/>
@@ -30207,13 +30207,13 @@
         <v>207</v>
       </c>
       <c r="B335" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1806</v>
+      </c>
+      <c r="D335" t="s">
         <v>1793</v>
-      </c>
-      <c r="C335" t="s">
-        <v>1807</v>
-      </c>
-      <c r="D335" t="s">
-        <v>1794</v>
       </c>
       <c r="F335" t="str">
         <f t="shared" si="4"/>
@@ -30225,13 +30225,13 @@
         <v>207</v>
       </c>
       <c r="B336" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="C336" t="s">
-        <v>1814</v>
+        <v>1809</v>
       </c>
       <c r="D336" t="s">
-        <v>1814</v>
+        <v>1809</v>
       </c>
       <c r="F336" t="str">
         <f t="shared" si="4"/>
@@ -30243,17 +30243,17 @@
         <v>207</v>
       </c>
       <c r="B337" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="C337" t="s">
-        <v>1815</v>
+        <v>1973</v>
       </c>
       <c r="D337" t="s">
-        <v>1815</v>
+        <v>1973</v>
       </c>
       <c r="F337" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "altres_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera Pn &gt; 70 kW", descripcio_es: "Caldera Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "altres_pn_major_70", sistema_element: "climatitzacio", descripcio_ca: "Caldera Pn &amp;gt; 70 kW", descripcio_es: "Caldera Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="338" spans="1:6" x14ac:dyDescent="0.2">
@@ -30261,13 +30261,13 @@
         <v>207</v>
       </c>
       <c r="B338" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="C338" t="s">
-        <v>1816</v>
+        <v>1810</v>
       </c>
       <c r="D338" t="s">
-        <v>1818</v>
+        <v>1812</v>
       </c>
       <c r="F338" t="str">
         <f t="shared" si="4"/>
@@ -30279,13 +30279,13 @@
         <v>207</v>
       </c>
       <c r="B339" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="C339" t="s">
-        <v>1817</v>
+        <v>1811</v>
       </c>
       <c r="D339" t="s">
-        <v>1819</v>
+        <v>1813</v>
       </c>
       <c r="F339" t="str">
         <f t="shared" si="4"/>
@@ -30297,13 +30297,13 @@
         <v>207</v>
       </c>
       <c r="B340" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="C340" t="s">
-        <v>1825</v>
+        <v>1815</v>
       </c>
       <c r="D340" t="s">
-        <v>1820</v>
+        <v>1814</v>
       </c>
       <c r="F340" t="str">
         <f t="shared" si="4"/>
@@ -30315,17 +30315,17 @@
         <v>207</v>
       </c>
       <c r="B341" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C341" t="s">
-        <v>1821</v>
+        <v>1964</v>
       </c>
       <c r="D341" t="s">
-        <v>1828</v>
+        <v>1965</v>
       </c>
       <c r="F341" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización autónomo 12 kW &lt; Pn ≤ 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom 12 kW &amp;lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización autónomo 12 kW &amp;lt; Pn ≤ 70 kW")</v>
       </c>
     </row>
     <row r="342" spans="1:6" x14ac:dyDescent="0.2">
@@ -30333,17 +30333,17 @@
         <v>207</v>
       </c>
       <c r="B342" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C342" t="s">
-        <v>1823</v>
+        <v>1966</v>
       </c>
       <c r="D342" t="s">
-        <v>1829</v>
+        <v>1968</v>
       </c>
       <c r="F342" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración 12 kW &lt; Pn ≤ 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració 12 kW &amp;lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración 12 kW &amp;lt; Pn ≤ 70 kW")</v>
       </c>
     </row>
     <row r="343" spans="1:6" x14ac:dyDescent="0.2">
@@ -30351,17 +30351,17 @@
         <v>207</v>
       </c>
       <c r="B343" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C343" t="s">
-        <v>1826</v>
+        <v>1967</v>
       </c>
       <c r="D343" t="s">
-        <v>1832</v>
+        <v>1969</v>
       </c>
       <c r="F343" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor 12 kW &lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor 12 kW &lt; Pn ≤ 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_12_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor 12 kW &amp;lt; Pn ≤ 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor 12 kW &amp;lt; Pn ≤ 70 kW")</v>
       </c>
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.2">
@@ -30369,17 +30369,17 @@
         <v>207</v>
       </c>
       <c r="B344" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C344" t="s">
-        <v>1822</v>
+        <v>1974</v>
       </c>
       <c r="D344" t="s">
-        <v>1831</v>
+        <v>1977</v>
       </c>
       <c r="F344" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom Pn &gt; 70 kW", descripcio_es: "Sistema de climatización autónomo Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_autonoms", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització autònom Pn &amp;gt; 70 kW", descripcio_es: "Sistema de climatización autónomo Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="345" spans="1:6" x14ac:dyDescent="0.2">
@@ -30387,17 +30387,17 @@
         <v>207</v>
       </c>
       <c r="B345" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="C345" t="s">
-        <v>1824</v>
+        <v>1975</v>
       </c>
       <c r="D345" t="s">
-        <v>1830</v>
+        <v>1978</v>
       </c>
       <c r="F345" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració Pn &gt; 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_torres", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb torre de refrigeració Pn &amp;gt; 70 kW", descripcio_es: "Sistema de climatización con torre de refrigeración Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.2">
@@ -30405,17 +30405,17 @@
         <v>207</v>
       </c>
       <c r="B346" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="C346" t="s">
-        <v>1827</v>
+        <v>1976</v>
       </c>
       <c r="D346" t="s">
-        <v>1833</v>
+        <v>1979</v>
       </c>
       <c r="F346" t="str">
         <f t="shared" si="4"/>
-        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor Pn &gt; 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor Pn &gt; 70 kW")</v>
+        <v>ElementPredefinit.create(nom_element: "clima_pn_major_70_recuperador", sistema_element: "climatitzacio", descripcio_ca: "Sistema de climatització amb recuperació de calor Pn &amp;gt; 70 kW", descripcio_es: "Sistema de climatización con recuperación de calor Pn &amp;gt; 70 kW")</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.2">
@@ -30423,13 +30423,13 @@
         <v>162</v>
       </c>
       <c r="B347" t="s">
-        <v>1834</v>
+        <v>1816</v>
       </c>
       <c r="C347" t="s">
-        <v>1840</v>
+        <v>1822</v>
       </c>
       <c r="D347" t="s">
-        <v>1835</v>
+        <v>1817</v>
       </c>
       <c r="F347" t="str">
         <f t="shared" si="4"/>
@@ -30441,13 +30441,13 @@
         <v>162</v>
       </c>
       <c r="B348" t="s">
-        <v>1836</v>
+        <v>1818</v>
       </c>
       <c r="C348" t="s">
-        <v>1841</v>
+        <v>1823</v>
       </c>
       <c r="D348" t="s">
-        <v>1838</v>
+        <v>1820</v>
       </c>
       <c r="F348" t="str">
         <f t="shared" si="4"/>
@@ -30459,13 +30459,13 @@
         <v>162</v>
       </c>
       <c r="B349" t="s">
-        <v>1837</v>
+        <v>1819</v>
       </c>
       <c r="C349" t="s">
-        <v>1842</v>
+        <v>1824</v>
       </c>
       <c r="D349" t="s">
-        <v>1839</v>
+        <v>1821</v>
       </c>
       <c r="F349" t="str">
         <f t="shared" si="4"/>
@@ -30477,13 +30477,13 @@
         <v>396</v>
       </c>
       <c r="B350" t="s">
-        <v>1843</v>
+        <v>1825</v>
       </c>
       <c r="C350" t="s">
-        <v>1868</v>
+        <v>1850</v>
       </c>
       <c r="D350" t="s">
-        <v>1844</v>
+        <v>1826</v>
       </c>
       <c r="F350" t="str">
         <f t="shared" si="4"/>
@@ -30495,13 +30495,13 @@
         <v>396</v>
       </c>
       <c r="B351" t="s">
-        <v>1845</v>
+        <v>1827</v>
       </c>
       <c r="C351" t="s">
-        <v>1869</v>
+        <v>1851</v>
       </c>
       <c r="D351" t="s">
-        <v>1846</v>
+        <v>1828</v>
       </c>
       <c r="F351" t="str">
         <f t="shared" si="4"/>
@@ -30513,13 +30513,13 @@
         <v>396</v>
       </c>
       <c r="B352" t="s">
-        <v>1847</v>
+        <v>1829</v>
       </c>
       <c r="C352" t="s">
-        <v>1870</v>
+        <v>1852</v>
       </c>
       <c r="D352" t="s">
-        <v>1848</v>
+        <v>1830</v>
       </c>
       <c r="F352" t="str">
         <f t="shared" si="4"/>
@@ -30531,13 +30531,13 @@
         <v>396</v>
       </c>
       <c r="B353" t="s">
-        <v>1849</v>
+        <v>1831</v>
       </c>
       <c r="C353" t="s">
-        <v>1871</v>
+        <v>1853</v>
       </c>
       <c r="D353" t="s">
-        <v>1850</v>
+        <v>1832</v>
       </c>
       <c r="F353" t="str">
         <f t="shared" si="4"/>
@@ -30549,13 +30549,13 @@
         <v>396</v>
       </c>
       <c r="B354" t="s">
-        <v>1851</v>
+        <v>1833</v>
       </c>
       <c r="C354" t="s">
-        <v>1872</v>
+        <v>1854</v>
       </c>
       <c r="D354" t="s">
-        <v>1852</v>
+        <v>1834</v>
       </c>
       <c r="F354" t="str">
         <f t="shared" ref="F354:F404" si="5">"ElementPredefinit.create(nom_element: """&amp;B354&amp;""", sistema_element: """&amp;A354&amp;""", descripcio_ca: """&amp;C354&amp;""", descripcio_es: """&amp;D354&amp;""")"</f>
@@ -30567,13 +30567,13 @@
         <v>396</v>
       </c>
       <c r="B355" t="s">
-        <v>1853</v>
+        <v>1835</v>
       </c>
       <c r="C355" t="s">
-        <v>1868</v>
+        <v>1850</v>
       </c>
       <c r="D355" t="s">
-        <v>1844</v>
+        <v>1826</v>
       </c>
       <c r="F355" t="str">
         <f t="shared" si="5"/>
@@ -30585,13 +30585,13 @@
         <v>396</v>
       </c>
       <c r="B356" t="s">
-        <v>1854</v>
+        <v>1836</v>
       </c>
       <c r="C356" t="s">
-        <v>1869</v>
+        <v>1851</v>
       </c>
       <c r="D356" t="s">
-        <v>1846</v>
+        <v>1828</v>
       </c>
       <c r="F356" t="str">
         <f t="shared" si="5"/>
@@ -30603,13 +30603,13 @@
         <v>396</v>
       </c>
       <c r="B357" t="s">
-        <v>1855</v>
+        <v>1837</v>
       </c>
       <c r="C357" t="s">
-        <v>1870</v>
+        <v>1852</v>
       </c>
       <c r="D357" t="s">
-        <v>1848</v>
+        <v>1830</v>
       </c>
       <c r="F357" t="str">
         <f t="shared" si="5"/>
@@ -30621,13 +30621,13 @@
         <v>396</v>
       </c>
       <c r="B358" t="s">
-        <v>1856</v>
+        <v>1838</v>
       </c>
       <c r="C358" t="s">
-        <v>1871</v>
+        <v>1853</v>
       </c>
       <c r="D358" t="s">
-        <v>1850</v>
+        <v>1832</v>
       </c>
       <c r="F358" t="str">
         <f t="shared" si="5"/>
@@ -30639,13 +30639,13 @@
         <v>396</v>
       </c>
       <c r="B359" t="s">
-        <v>1857</v>
+        <v>1839</v>
       </c>
       <c r="C359" t="s">
-        <v>1872</v>
+        <v>1854</v>
       </c>
       <c r="D359" t="s">
-        <v>1852</v>
+        <v>1834</v>
       </c>
       <c r="F359" t="str">
         <f t="shared" si="5"/>
@@ -30657,13 +30657,13 @@
         <v>396</v>
       </c>
       <c r="B360" t="s">
-        <v>1858</v>
+        <v>1840</v>
       </c>
       <c r="C360" t="s">
-        <v>1868</v>
+        <v>1850</v>
       </c>
       <c r="D360" t="s">
-        <v>1844</v>
+        <v>1826</v>
       </c>
       <c r="F360" t="str">
         <f t="shared" si="5"/>
@@ -30675,13 +30675,13 @@
         <v>396</v>
       </c>
       <c r="B361" t="s">
-        <v>1859</v>
+        <v>1841</v>
       </c>
       <c r="C361" t="s">
-        <v>1869</v>
+        <v>1851</v>
       </c>
       <c r="D361" t="s">
-        <v>1846</v>
+        <v>1828</v>
       </c>
       <c r="F361" t="str">
         <f t="shared" si="5"/>
@@ -30693,13 +30693,13 @@
         <v>396</v>
       </c>
       <c r="B362" t="s">
-        <v>1860</v>
+        <v>1842</v>
       </c>
       <c r="C362" t="s">
-        <v>1870</v>
+        <v>1852</v>
       </c>
       <c r="D362" t="s">
-        <v>1848</v>
+        <v>1830</v>
       </c>
       <c r="F362" t="str">
         <f t="shared" si="5"/>
@@ -30711,13 +30711,13 @@
         <v>396</v>
       </c>
       <c r="B363" t="s">
-        <v>1861</v>
+        <v>1843</v>
       </c>
       <c r="C363" t="s">
-        <v>1871</v>
+        <v>1853</v>
       </c>
       <c r="D363" t="s">
-        <v>1850</v>
+        <v>1832</v>
       </c>
       <c r="F363" t="str">
         <f t="shared" si="5"/>
@@ -30729,13 +30729,13 @@
         <v>396</v>
       </c>
       <c r="B364" t="s">
-        <v>1862</v>
+        <v>1844</v>
       </c>
       <c r="C364" t="s">
-        <v>1872</v>
+        <v>1854</v>
       </c>
       <c r="D364" t="s">
-        <v>1852</v>
+        <v>1834</v>
       </c>
       <c r="F364" t="str">
         <f t="shared" si="5"/>
@@ -30747,13 +30747,13 @@
         <v>396</v>
       </c>
       <c r="B365" t="s">
-        <v>1863</v>
+        <v>1845</v>
       </c>
       <c r="C365" t="s">
-        <v>1868</v>
+        <v>1850</v>
       </c>
       <c r="D365" t="s">
-        <v>1844</v>
+        <v>1826</v>
       </c>
       <c r="F365" t="str">
         <f t="shared" si="5"/>
@@ -30765,13 +30765,13 @@
         <v>396</v>
       </c>
       <c r="B366" t="s">
-        <v>1864</v>
+        <v>1846</v>
       </c>
       <c r="C366" t="s">
-        <v>1869</v>
+        <v>1851</v>
       </c>
       <c r="D366" t="s">
-        <v>1846</v>
+        <v>1828</v>
       </c>
       <c r="F366" t="str">
         <f t="shared" si="5"/>
@@ -30783,13 +30783,13 @@
         <v>396</v>
       </c>
       <c r="B367" t="s">
-        <v>1865</v>
+        <v>1847</v>
       </c>
       <c r="C367" t="s">
-        <v>1870</v>
+        <v>1852</v>
       </c>
       <c r="D367" t="s">
-        <v>1848</v>
+        <v>1830</v>
       </c>
       <c r="F367" t="str">
         <f t="shared" si="5"/>
@@ -30801,13 +30801,13 @@
         <v>396</v>
       </c>
       <c r="B368" t="s">
-        <v>1866</v>
+        <v>1848</v>
       </c>
       <c r="C368" t="s">
-        <v>1871</v>
+        <v>1853</v>
       </c>
       <c r="D368" t="s">
-        <v>1850</v>
+        <v>1832</v>
       </c>
       <c r="F368" t="str">
         <f t="shared" si="5"/>
@@ -30819,13 +30819,13 @@
         <v>396</v>
       </c>
       <c r="B369" t="s">
-        <v>1867</v>
+        <v>1849</v>
       </c>
       <c r="C369" t="s">
-        <v>1872</v>
+        <v>1854</v>
       </c>
       <c r="D369" t="s">
-        <v>1852</v>
+        <v>1834</v>
       </c>
       <c r="F369" t="str">
         <f t="shared" si="5"/>
@@ -30837,13 +30837,13 @@
         <v>462</v>
       </c>
       <c r="B370" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C370" t="s">
         <v>1873</v>
       </c>
-      <c r="C370" t="s">
-        <v>1891</v>
-      </c>
       <c r="D370" t="s">
-        <v>1874</v>
+        <v>1856</v>
       </c>
       <c r="F370" t="str">
         <f t="shared" si="5"/>
@@ -30855,13 +30855,13 @@
         <v>462</v>
       </c>
       <c r="B371" t="s">
-        <v>1875</v>
+        <v>1857</v>
       </c>
       <c r="C371" t="s">
-        <v>1892</v>
+        <v>1874</v>
       </c>
       <c r="D371" t="s">
-        <v>1876</v>
+        <v>1858</v>
       </c>
       <c r="F371" t="str">
         <f t="shared" si="5"/>
@@ -30873,13 +30873,13 @@
         <v>462</v>
       </c>
       <c r="B372" t="s">
-        <v>1877</v>
+        <v>1859</v>
       </c>
       <c r="C372" t="s">
-        <v>1893</v>
+        <v>1875</v>
       </c>
       <c r="D372" t="s">
-        <v>1878</v>
+        <v>1860</v>
       </c>
       <c r="F372" t="str">
         <f t="shared" si="5"/>
@@ -30891,13 +30891,13 @@
         <v>462</v>
       </c>
       <c r="B373" t="s">
-        <v>1879</v>
+        <v>1861</v>
       </c>
       <c r="C373" t="s">
-        <v>1894</v>
+        <v>1876</v>
       </c>
       <c r="D373" t="s">
-        <v>1880</v>
+        <v>1862</v>
       </c>
       <c r="F373" t="str">
         <f t="shared" si="5"/>
@@ -30909,13 +30909,13 @@
         <v>462</v>
       </c>
       <c r="B374" t="s">
-        <v>1881</v>
+        <v>1863</v>
       </c>
       <c r="C374" t="s">
-        <v>1895</v>
+        <v>1877</v>
       </c>
       <c r="D374" t="s">
-        <v>1882</v>
+        <v>1864</v>
       </c>
       <c r="F374" t="str">
         <f t="shared" si="5"/>
@@ -30927,13 +30927,13 @@
         <v>462</v>
       </c>
       <c r="B375" t="s">
-        <v>1883</v>
+        <v>1865</v>
       </c>
       <c r="C375" t="s">
-        <v>1896</v>
+        <v>1878</v>
       </c>
       <c r="D375" t="s">
-        <v>1884</v>
+        <v>1866</v>
       </c>
       <c r="F375" t="str">
         <f t="shared" si="5"/>
@@ -30945,13 +30945,13 @@
         <v>462</v>
       </c>
       <c r="B376" t="s">
-        <v>1885</v>
+        <v>1867</v>
       </c>
       <c r="C376" t="s">
-        <v>1897</v>
+        <v>1879</v>
       </c>
       <c r="D376" t="s">
-        <v>1886</v>
+        <v>1868</v>
       </c>
       <c r="F376" t="str">
         <f t="shared" si="5"/>
@@ -30963,13 +30963,13 @@
         <v>462</v>
       </c>
       <c r="B377" t="s">
-        <v>1887</v>
+        <v>1869</v>
       </c>
       <c r="C377" t="s">
-        <v>1898</v>
+        <v>1880</v>
       </c>
       <c r="D377" t="s">
-        <v>1888</v>
+        <v>1870</v>
       </c>
       <c r="F377" t="str">
         <f t="shared" si="5"/>
@@ -30981,13 +30981,13 @@
         <v>462</v>
       </c>
       <c r="B378" t="s">
-        <v>1889</v>
+        <v>1871</v>
       </c>
       <c r="C378" t="s">
-        <v>1899</v>
+        <v>1881</v>
       </c>
       <c r="D378" t="s">
-        <v>1890</v>
+        <v>1872</v>
       </c>
       <c r="F378" t="str">
         <f t="shared" si="5"/>
@@ -30996,16 +30996,16 @@
     </row>
     <row r="379" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>1911</v>
+        <v>1893</v>
       </c>
       <c r="B379" t="s">
-        <v>1900</v>
+        <v>1882</v>
       </c>
       <c r="C379" t="s">
-        <v>1910</v>
+        <v>1892</v>
       </c>
       <c r="D379" t="s">
-        <v>1905</v>
+        <v>1887</v>
       </c>
       <c r="F379" t="str">
         <f t="shared" si="5"/>
@@ -31014,16 +31014,16 @@
     </row>
     <row r="380" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>1911</v>
+        <v>1893</v>
       </c>
       <c r="B380" t="s">
-        <v>1901</v>
+        <v>1883</v>
       </c>
       <c r="C380" t="s">
-        <v>1908</v>
+        <v>1890</v>
       </c>
       <c r="D380" t="s">
-        <v>1902</v>
+        <v>1884</v>
       </c>
       <c r="F380" t="str">
         <f t="shared" si="5"/>
@@ -31032,16 +31032,16 @@
     </row>
     <row r="381" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>1911</v>
+        <v>1893</v>
       </c>
       <c r="B381" t="s">
-        <v>1903</v>
+        <v>1885</v>
       </c>
       <c r="C381" t="s">
-        <v>1909</v>
+        <v>1891</v>
       </c>
       <c r="D381" t="s">
-        <v>1906</v>
+        <v>1888</v>
       </c>
       <c r="F381" t="str">
         <f t="shared" si="5"/>
@@ -31050,16 +31050,16 @@
     </row>
     <row r="382" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>1911</v>
+        <v>1893</v>
       </c>
       <c r="B382" t="s">
-        <v>1904</v>
+        <v>1886</v>
       </c>
       <c r="C382" t="s">
-        <v>1907</v>
+        <v>1889</v>
       </c>
       <c r="D382" t="s">
-        <v>1907</v>
+        <v>1889</v>
       </c>
       <c r="F382" t="str">
         <f t="shared" si="5"/>
@@ -31071,13 +31071,13 @@
         <v>600</v>
       </c>
       <c r="B383" t="s">
-        <v>1912</v>
+        <v>1894</v>
       </c>
       <c r="C383" t="s">
-        <v>1934</v>
+        <v>1916</v>
       </c>
       <c r="D383" t="s">
-        <v>1913</v>
+        <v>1895</v>
       </c>
       <c r="F383" t="str">
         <f t="shared" si="5"/>
@@ -31089,13 +31089,13 @@
         <v>600</v>
       </c>
       <c r="B384" t="s">
-        <v>1914</v>
+        <v>1896</v>
       </c>
       <c r="C384" t="s">
-        <v>1935</v>
+        <v>1917</v>
       </c>
       <c r="D384" t="s">
-        <v>1915</v>
+        <v>1897</v>
       </c>
       <c r="F384" t="str">
         <f t="shared" si="5"/>
@@ -31107,13 +31107,13 @@
         <v>600</v>
       </c>
       <c r="B385" t="s">
-        <v>1916</v>
+        <v>1898</v>
       </c>
       <c r="C385" t="s">
-        <v>1936</v>
+        <v>1918</v>
       </c>
       <c r="D385" t="s">
-        <v>1917</v>
+        <v>1899</v>
       </c>
       <c r="F385" t="str">
         <f t="shared" si="5"/>
@@ -31125,13 +31125,13 @@
         <v>600</v>
       </c>
       <c r="B386" t="s">
-        <v>1918</v>
+        <v>1900</v>
       </c>
       <c r="C386" t="s">
-        <v>1937</v>
+        <v>1919</v>
       </c>
       <c r="D386" t="s">
-        <v>1919</v>
+        <v>1901</v>
       </c>
       <c r="F386" t="str">
         <f t="shared" si="5"/>
@@ -31143,13 +31143,13 @@
         <v>600</v>
       </c>
       <c r="B387" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C387" t="s">
         <v>1920</v>
       </c>
-      <c r="C387" t="s">
-        <v>1938</v>
-      </c>
       <c r="D387" t="s">
-        <v>1921</v>
+        <v>1903</v>
       </c>
       <c r="F387" t="str">
         <f t="shared" si="5"/>
@@ -31161,13 +31161,13 @@
         <v>600</v>
       </c>
       <c r="B388" t="s">
-        <v>1922</v>
+        <v>1904</v>
       </c>
       <c r="C388" t="s">
-        <v>1939</v>
+        <v>1921</v>
       </c>
       <c r="D388" t="s">
-        <v>1923</v>
+        <v>1905</v>
       </c>
       <c r="F388" t="str">
         <f t="shared" si="5"/>
@@ -31179,13 +31179,13 @@
         <v>600</v>
       </c>
       <c r="B389" t="s">
-        <v>1924</v>
+        <v>1906</v>
       </c>
       <c r="C389" t="s">
-        <v>1940</v>
+        <v>1922</v>
       </c>
       <c r="D389" t="s">
-        <v>1925</v>
+        <v>1907</v>
       </c>
       <c r="F389" t="str">
         <f t="shared" si="5"/>
@@ -31197,13 +31197,13 @@
         <v>600</v>
       </c>
       <c r="B390" t="s">
-        <v>1926</v>
+        <v>1908</v>
       </c>
       <c r="C390" t="s">
-        <v>1941</v>
+        <v>1923</v>
       </c>
       <c r="D390" t="s">
-        <v>1927</v>
+        <v>1909</v>
       </c>
       <c r="F390" t="str">
         <f t="shared" si="5"/>
@@ -31215,13 +31215,13 @@
         <v>600</v>
       </c>
       <c r="B391" t="s">
-        <v>1928</v>
+        <v>1910</v>
       </c>
       <c r="C391" t="s">
-        <v>1942</v>
+        <v>1924</v>
       </c>
       <c r="D391" t="s">
-        <v>1929</v>
+        <v>1911</v>
       </c>
       <c r="F391" t="str">
         <f t="shared" si="5"/>
@@ -31233,13 +31233,13 @@
         <v>600</v>
       </c>
       <c r="B392" t="s">
-        <v>1930</v>
+        <v>1912</v>
       </c>
       <c r="C392" t="s">
-        <v>1943</v>
+        <v>1925</v>
       </c>
       <c r="D392" t="s">
-        <v>1931</v>
+        <v>1913</v>
       </c>
       <c r="F392" t="str">
         <f t="shared" si="5"/>
@@ -31251,13 +31251,13 @@
         <v>600</v>
       </c>
       <c r="B393" t="s">
-        <v>1932</v>
+        <v>1914</v>
       </c>
       <c r="C393" t="s">
-        <v>1944</v>
+        <v>1926</v>
       </c>
       <c r="D393" t="s">
-        <v>1933</v>
+        <v>1915</v>
       </c>
       <c r="F393" t="str">
         <f t="shared" si="5"/>
@@ -31269,13 +31269,13 @@
         <v>633</v>
       </c>
       <c r="B394" t="s">
-        <v>1945</v>
+        <v>1927</v>
       </c>
       <c r="C394" t="s">
-        <v>1972</v>
+        <v>1954</v>
       </c>
       <c r="D394" t="s">
-        <v>1975</v>
+        <v>1957</v>
       </c>
       <c r="F394" t="str">
         <f t="shared" si="5"/>
@@ -31287,13 +31287,13 @@
         <v>633</v>
       </c>
       <c r="B395" t="s">
-        <v>1946</v>
+        <v>1928</v>
       </c>
       <c r="C395" t="s">
-        <v>1973</v>
+        <v>1955</v>
       </c>
       <c r="D395" t="s">
-        <v>1976</v>
+        <v>1958</v>
       </c>
       <c r="F395" t="str">
         <f t="shared" si="5"/>
@@ -31305,13 +31305,13 @@
         <v>633</v>
       </c>
       <c r="B396" t="s">
-        <v>1947</v>
+        <v>1929</v>
       </c>
       <c r="C396" t="s">
-        <v>1974</v>
+        <v>1956</v>
       </c>
       <c r="D396" t="s">
-        <v>1977</v>
+        <v>1959</v>
       </c>
       <c r="F396" t="str">
         <f t="shared" si="5"/>
@@ -31323,13 +31323,13 @@
         <v>633</v>
       </c>
       <c r="B397" t="s">
-        <v>1948</v>
+        <v>1930</v>
       </c>
       <c r="C397" t="s">
-        <v>1964</v>
+        <v>1946</v>
       </c>
       <c r="D397" t="s">
-        <v>1949</v>
+        <v>1931</v>
       </c>
       <c r="F397" t="str">
         <f t="shared" si="5"/>
@@ -31341,13 +31341,13 @@
         <v>633</v>
       </c>
       <c r="B398" t="s">
-        <v>1950</v>
+        <v>1932</v>
       </c>
       <c r="C398" t="s">
-        <v>1965</v>
+        <v>1947</v>
       </c>
       <c r="D398" t="s">
-        <v>1951</v>
+        <v>1933</v>
       </c>
       <c r="F398" t="str">
         <f t="shared" si="5"/>
@@ -31359,13 +31359,13 @@
         <v>633</v>
       </c>
       <c r="B399" t="s">
-        <v>1952</v>
+        <v>1934</v>
       </c>
       <c r="C399" t="s">
-        <v>1966</v>
+        <v>1948</v>
       </c>
       <c r="D399" t="s">
-        <v>1953</v>
+        <v>1935</v>
       </c>
       <c r="F399" t="str">
         <f t="shared" si="5"/>
@@ -31377,13 +31377,13 @@
         <v>633</v>
       </c>
       <c r="B400" t="s">
-        <v>1954</v>
+        <v>1936</v>
       </c>
       <c r="C400" t="s">
-        <v>1967</v>
+        <v>1949</v>
       </c>
       <c r="D400" t="s">
-        <v>1955</v>
+        <v>1937</v>
       </c>
       <c r="F400" t="str">
         <f t="shared" si="5"/>
@@ -31395,13 +31395,13 @@
         <v>633</v>
       </c>
       <c r="B401" t="s">
-        <v>1956</v>
+        <v>1938</v>
       </c>
       <c r="C401" t="s">
-        <v>1968</v>
+        <v>1950</v>
       </c>
       <c r="D401" t="s">
-        <v>1957</v>
+        <v>1939</v>
       </c>
       <c r="F401" t="str">
         <f t="shared" si="5"/>
@@ -31413,13 +31413,13 @@
         <v>633</v>
       </c>
       <c r="B402" t="s">
-        <v>1958</v>
+        <v>1940</v>
       </c>
       <c r="C402" t="s">
-        <v>1969</v>
+        <v>1951</v>
       </c>
       <c r="D402" t="s">
-        <v>1959</v>
+        <v>1941</v>
       </c>
       <c r="F402" t="str">
         <f t="shared" si="5"/>
@@ -31431,13 +31431,13 @@
         <v>633</v>
       </c>
       <c r="B403" t="s">
-        <v>1960</v>
+        <v>1942</v>
       </c>
       <c r="C403" t="s">
-        <v>1970</v>
+        <v>1952</v>
       </c>
       <c r="D403" t="s">
-        <v>1961</v>
+        <v>1943</v>
       </c>
       <c r="F403" t="str">
         <f t="shared" si="5"/>
@@ -31449,13 +31449,13 @@
         <v>633</v>
       </c>
       <c r="B404" t="s">
-        <v>1962</v>
+        <v>1944</v>
       </c>
       <c r="C404" t="s">
-        <v>1971</v>
+        <v>1953</v>
       </c>
       <c r="D404" t="s">
-        <v>1963</v>
+        <v>1945</v>
       </c>
       <c r="F404" t="str">
         <f t="shared" si="5"/>

</xml_diff>